<commit_message>
Epicas e historias de usuario corregida
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Epicas e historias de usuario _ Priorización.xlsx
+++ b/Fase 2/Evidencias Proyecto/Epicas e historias de usuario _ Priorización.xlsx
@@ -460,7 +460,7 @@
     <t>Horas Primer Sprint</t>
   </si>
   <si>
-    <t>E1H1</t>
+    <t>E01-H01: Visualización de datos personales y configuraciones de cuenta.</t>
   </si>
   <si>
     <t>SPRINT 2</t>
@@ -472,7 +472,7 @@
     <t>Horas Segundo Sprint</t>
   </si>
   <si>
-    <t>E1H2</t>
+    <t>E01-H02: Inicio de sesión en el sistema.</t>
   </si>
   <si>
     <t>SPRINT 3</t>
@@ -481,7 +481,7 @@
     <t>Horas Tercer Sprint</t>
   </si>
   <si>
-    <t>E1H3</t>
+    <t>E01-H03: Edición de perfil de usuario.</t>
   </si>
   <si>
     <t>SPRINT 4</t>
@@ -490,7 +490,7 @@
     <t>Horas Cuarto Sprint</t>
   </si>
   <si>
-    <t>E1H4</t>
+    <t>E01-H04: Visualización de datos personales para administradores.</t>
   </si>
   <si>
     <t>SPRINT 5</t>
@@ -499,7 +499,7 @@
     <t>Horas Quinto Sprint</t>
   </si>
   <si>
-    <t>E1H5</t>
+    <t>E01-H05: Gestión del estado de empleados por parte del administrador.</t>
   </si>
   <si>
     <t>SPRINT 6</t>
@@ -508,58 +508,58 @@
     <t>Horas Sexto Sprint</t>
   </si>
   <si>
-    <t>E2H1</t>
+    <t>E02-H01: Visualización de Productos Disponibles y No Disponibles</t>
   </si>
   <si>
-    <t>E2H2</t>
+    <t>E02-H02: Historial de Movimientos</t>
   </si>
   <si>
-    <t>E2H3</t>
+    <t>E02-H03: Registro de Entradas y Salidas de Inventario</t>
   </si>
   <si>
-    <t>E3H1</t>
+    <t>E03-H01: Reporte de Productos Más Vendidos</t>
   </si>
   <si>
-    <t>E3H2</t>
+    <t>E03-H02: Reporte de Productos Más Rentables</t>
   </si>
   <si>
-    <t>E3H3</t>
+    <t>E03-H03: Reporte de Productos Sin Movimiento</t>
   </si>
   <si>
-    <t>E3H4</t>
+    <t>E03-H04: Reporte del Estado de Productos (Crítico, Mínimo o Normal)</t>
   </si>
   <si>
-    <t>E3H5</t>
+    <t>E03-H05: Reporte de Productos en Merma</t>
   </si>
   <si>
-    <t>E4H1</t>
+    <t>E04-H01: Creación de Productos</t>
   </si>
   <si>
-    <t>E4H2</t>
+    <t>E04-H02: Edición de Productos</t>
   </si>
   <si>
-    <t>E4H3</t>
+    <t>E04-H03: Visualización de Productos</t>
   </si>
   <si>
-    <t>E4H4</t>
+    <t>E04-H04: Eliminación de Productos</t>
   </si>
   <si>
-    <t>E6H1</t>
+    <t>E06-H01: Interfaz Intuitiva con Filtros de Búsqueda</t>
   </si>
   <si>
-    <t>E5H2</t>
+    <t>E05-H02: Edición de Proveedores</t>
   </si>
   <si>
-    <t>E5H3</t>
+    <t>E05-H03: Eliminación de Proveedores</t>
   </si>
   <si>
-    <t>E5H4</t>
+    <t>E05-H04: Visualización de Proveedores</t>
   </si>
   <si>
-    <t>E5H1</t>
+    <t>E05-H01: Creación de Proveedores</t>
   </si>
   <si>
-    <t>E7H1</t>
+    <t>E7- H1: Integración y Exportación de Datos</t>
   </si>
   <si>
     <t>Para calcular el esfuerzo tomaremos como base la historia 16</t>
@@ -979,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="90">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1098,7 +1098,7 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="8" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
@@ -1130,11 +1130,17 @@
     </xf>
     <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="8" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="11" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="12" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="13" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1148,8 +1154,14 @@
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="4" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="12" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -1157,9 +1169,18 @@
     <xf borderId="8" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="8" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="4" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="11" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="13" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -33190,7 +33211,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.88"/>
+    <col customWidth="1" min="1" max="1" width="52.75"/>
     <col customWidth="1" min="2" max="3" width="11.38"/>
     <col customWidth="1" min="4" max="4" width="13.5"/>
     <col customWidth="1" min="5" max="5" width="14.25"/>
@@ -33368,7 +33389,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="58" t="s">
         <v>149</v>
       </c>
       <c r="B6" s="46">
@@ -33397,7 +33418,7 @@
         <f>Esfurezo!E7</f>
         <v>16.2</v>
       </c>
-      <c r="J6" s="58" t="s">
+      <c r="J6" s="59" t="s">
         <v>150</v>
       </c>
       <c r="L6" s="51"/>
@@ -33444,7 +33465,7 @@
         <f>Esfurezo!E8</f>
         <v>10.2</v>
       </c>
-      <c r="J7" s="59" t="s">
+      <c r="J7" s="60" t="s">
         <v>153</v>
       </c>
       <c r="L7" s="51"/>
@@ -33462,7 +33483,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="61" t="s">
         <v>155</v>
       </c>
       <c r="B8" s="46">
@@ -33491,7 +33512,7 @@
         <f>Esfurezo!E9</f>
         <v>16.2</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="62" t="s">
         <v>156</v>
       </c>
       <c r="L8" s="51"/>
@@ -33531,7 +33552,7 @@
       <c r="G9" s="46">
         <v>13.0</v>
       </c>
-      <c r="H9" s="61">
+      <c r="H9" s="63">
         <v>1.0</v>
       </c>
       <c r="I9" s="47">
@@ -33546,29 +33567,29 @@
       <c r="O9" s="56"/>
     </row>
     <row r="10">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="62">
+      <c r="B10" s="64">
         <v>7.0</v>
       </c>
-      <c r="C10" s="63">
+      <c r="C10" s="65">
         <v>13.0</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="65">
         <v>8.0</v>
       </c>
-      <c r="E10" s="63">
+      <c r="E10" s="65">
         <v>21.0</v>
       </c>
       <c r="F10" s="48">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="G10" s="63">
+      <c r="G10" s="65">
         <v>13.0</v>
       </c>
-      <c r="H10" s="61">
+      <c r="H10" s="63">
         <v>2.0</v>
       </c>
       <c r="I10" s="47">
@@ -33583,7 +33604,7 @@
       <c r="O10" s="25"/>
     </row>
     <row r="11">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="61" t="s">
         <v>160</v>
       </c>
       <c r="B11" s="46">
@@ -33605,7 +33626,7 @@
       <c r="G11" s="46">
         <v>21.0</v>
       </c>
-      <c r="H11" s="61">
+      <c r="H11" s="63">
         <v>3.0</v>
       </c>
       <c r="I11" s="47">
@@ -33620,7 +33641,7 @@
       <c r="O11" s="33"/>
     </row>
     <row r="12">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="66" t="s">
         <v>161</v>
       </c>
       <c r="B12" s="46">
@@ -33642,7 +33663,7 @@
       <c r="G12" s="46">
         <v>21.0</v>
       </c>
-      <c r="H12" s="64">
+      <c r="H12" s="67">
         <v>1.0</v>
       </c>
       <c r="I12" s="47">
@@ -33656,7 +33677,7 @@
       <c r="O12" s="33"/>
     </row>
     <row r="13">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="58" t="s">
         <v>162</v>
       </c>
       <c r="B13" s="46">
@@ -33678,7 +33699,7 @@
       <c r="G13" s="46">
         <v>8.0</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="67">
         <v>5.0</v>
       </c>
       <c r="I13" s="47">
@@ -33693,7 +33714,7 @@
       <c r="O13" s="33"/>
     </row>
     <row r="14">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="58" t="s">
         <v>163</v>
       </c>
       <c r="B14" s="46">
@@ -33715,7 +33736,7 @@
       <c r="G14" s="46">
         <v>5.0</v>
       </c>
-      <c r="H14" s="64">
+      <c r="H14" s="67">
         <v>2.0</v>
       </c>
       <c r="I14" s="47">
@@ -33730,7 +33751,7 @@
       <c r="O14" s="33"/>
     </row>
     <row r="15">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="58" t="s">
         <v>164</v>
       </c>
       <c r="B15" s="46">
@@ -33752,7 +33773,7 @@
       <c r="G15" s="46">
         <v>13.0</v>
       </c>
-      <c r="H15" s="64">
+      <c r="H15" s="67">
         <v>4.0</v>
       </c>
       <c r="I15" s="47">
@@ -33763,7 +33784,7 @@
       <c r="O15" s="33"/>
     </row>
     <row r="16">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="68" t="s">
         <v>165</v>
       </c>
       <c r="B16" s="46">
@@ -33785,7 +33806,7 @@
       <c r="G16" s="46">
         <v>8.0</v>
       </c>
-      <c r="H16" s="64">
+      <c r="H16" s="67">
         <v>3.0</v>
       </c>
       <c r="I16" s="47">
@@ -33797,10 +33818,10 @@
       <c r="O16" s="33"/>
     </row>
     <row r="17">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="B17" s="65">
+      <c r="B17" s="69">
         <v>14.0</v>
       </c>
       <c r="C17" s="46">
@@ -33819,7 +33840,7 @@
       <c r="G17" s="46">
         <v>8.0</v>
       </c>
-      <c r="H17" s="66">
+      <c r="H17" s="70">
         <v>4.0</v>
       </c>
       <c r="I17" s="47">
@@ -33828,7 +33849,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="58" t="s">
         <v>167</v>
       </c>
       <c r="B18" s="46">
@@ -33850,7 +33871,7 @@
       <c r="G18" s="46">
         <v>8.0</v>
       </c>
-      <c r="H18" s="66">
+      <c r="H18" s="70">
         <v>3.0</v>
       </c>
       <c r="I18" s="47">
@@ -33859,7 +33880,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="58" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="46">
@@ -33881,7 +33902,7 @@
       <c r="G19" s="46">
         <v>3.0</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="70">
         <v>1.0</v>
       </c>
       <c r="I19" s="47">
@@ -33894,7 +33915,7 @@
       <c r="O19" s="33"/>
     </row>
     <row r="20">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="58" t="s">
         <v>169</v>
       </c>
       <c r="B20" s="46">
@@ -33916,7 +33937,7 @@
       <c r="G20" s="46">
         <v>3.0</v>
       </c>
-      <c r="H20" s="66">
+      <c r="H20" s="70">
         <v>2.0</v>
       </c>
       <c r="I20" s="47">
@@ -33929,7 +33950,7 @@
       <c r="O20" s="33"/>
     </row>
     <row r="21">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="71" t="s">
         <v>170</v>
       </c>
       <c r="B21" s="46">
@@ -33951,20 +33972,20 @@
       <c r="G21" s="46">
         <v>8.0</v>
       </c>
-      <c r="H21" s="66">
+      <c r="H21" s="70">
         <v>5.0</v>
       </c>
       <c r="I21" s="47">
         <f>Esfurezo!E26</f>
         <v>16.2</v>
       </c>
-      <c r="L21" s="67"/>
+      <c r="L21" s="72"/>
       <c r="M21" s="33"/>
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
     </row>
     <row r="22">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="73" t="s">
         <v>171</v>
       </c>
       <c r="B22" s="46">
@@ -33986,7 +34007,7 @@
       <c r="G22" s="46">
         <v>3.0</v>
       </c>
-      <c r="H22" s="68">
+      <c r="H22" s="74">
         <v>3.0</v>
       </c>
       <c r="I22" s="47">
@@ -34021,7 +34042,7 @@
       <c r="G23" s="46">
         <v>5.0</v>
       </c>
-      <c r="H23" s="68">
+      <c r="H23" s="74">
         <v>2.0</v>
       </c>
       <c r="I23" s="47">
@@ -34037,7 +34058,7 @@
       <c r="A24" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="B24" s="65">
+      <c r="B24" s="69">
         <v>21.0</v>
       </c>
       <c r="C24" s="46">
@@ -34056,7 +34077,7 @@
       <c r="G24" s="46">
         <v>8.0</v>
       </c>
-      <c r="H24" s="68">
+      <c r="H24" s="74">
         <v>1.0</v>
       </c>
       <c r="I24" s="47">
@@ -34069,7 +34090,7 @@
       <c r="O24" s="33"/>
     </row>
     <row r="25">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="61" t="s">
         <v>174</v>
       </c>
       <c r="B25" s="46">
@@ -34091,7 +34112,7 @@
       <c r="G25" s="46">
         <v>3.0</v>
       </c>
-      <c r="H25" s="68">
+      <c r="H25" s="74">
         <v>4.0</v>
       </c>
       <c r="I25" s="47">
@@ -34104,7 +34125,7 @@
       <c r="O25" s="33"/>
     </row>
     <row r="26">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="75" t="s">
         <v>175</v>
       </c>
       <c r="B26" s="46">
@@ -34126,7 +34147,7 @@
       <c r="G26" s="46">
         <v>13.0</v>
       </c>
-      <c r="H26" s="69">
+      <c r="H26" s="76">
         <v>1.0</v>
       </c>
       <c r="I26" s="47">
@@ -34144,9 +34165,9 @@
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
-      <c r="F27" s="70"/>
+      <c r="F27" s="77"/>
       <c r="G27" s="34"/>
-      <c r="H27" s="71"/>
+      <c r="H27" s="78"/>
       <c r="I27" s="34"/>
       <c r="J27" s="33"/>
       <c r="K27" s="33"/>
@@ -37117,56 +37138,56 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="D1" s="72"/>
+      <c r="D1" s="79"/>
     </row>
     <row r="2">
-      <c r="A2" s="73"/>
-      <c r="B2" s="74" t="s">
+      <c r="A2" s="80"/>
+      <c r="B2" s="81" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3">
-      <c r="A3" s="73"/>
-      <c r="B3" s="74" t="s">
+      <c r="A3" s="80"/>
+      <c r="B3" s="81" t="s">
         <v>177</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="81" t="s">
         <v>178</v>
       </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
     </row>
     <row r="4">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="82" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="84" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="75" t="s">
+      <c r="E4" s="82" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="78">
+      <c r="A5" s="85">
         <v>1.0</v>
       </c>
       <c r="B5" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="86">
         <v>8.0</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E5" s="47">
@@ -37175,16 +37196,16 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="78">
+      <c r="A6" s="85">
         <v>2.0</v>
       </c>
       <c r="B6" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="C6" s="79">
+      <c r="C6" s="86">
         <v>5.0</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="87" t="s">
         <v>185</v>
       </c>
       <c r="E6" s="47">
@@ -37193,16 +37214,16 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="78">
+      <c r="A7" s="85">
         <v>3.0</v>
       </c>
       <c r="B7" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="86">
         <v>8.0</v>
       </c>
-      <c r="D7" s="80" t="s">
+      <c r="D7" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E7" s="47">
@@ -37211,16 +37232,16 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="78">
+      <c r="A8" s="85">
         <v>4.0</v>
       </c>
       <c r="B8" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="79">
+      <c r="C8" s="86">
         <v>5.0</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="87" t="s">
         <v>185</v>
       </c>
       <c r="E8" s="47">
@@ -37229,16 +37250,16 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="78">
+      <c r="A9" s="85">
         <v>5.0</v>
       </c>
       <c r="B9" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="86">
         <v>8.0</v>
       </c>
-      <c r="D9" s="80" t="s">
+      <c r="D9" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E9" s="47">
@@ -37247,7 +37268,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="78">
+      <c r="A10" s="85">
         <v>6.0</v>
       </c>
       <c r="B10" s="51" t="s">
@@ -37256,7 +37277,7 @@
       <c r="C10" s="47">
         <v>13.0</v>
       </c>
-      <c r="D10" s="80" t="s">
+      <c r="D10" s="87" t="s">
         <v>190</v>
       </c>
       <c r="E10" s="47">
@@ -37265,16 +37286,16 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="78">
+      <c r="A11" s="85">
         <v>7.0</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="88" t="s">
         <v>191</v>
       </c>
-      <c r="C11" s="82">
+      <c r="C11" s="89">
         <v>13.0</v>
       </c>
-      <c r="D11" s="80" t="s">
+      <c r="D11" s="87" t="s">
         <v>190</v>
       </c>
       <c r="E11" s="47">
@@ -37283,16 +37304,16 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="78">
+      <c r="A12" s="85">
         <v>8.0</v>
       </c>
       <c r="B12" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="C12" s="79">
+      <c r="C12" s="86">
         <v>21.0</v>
       </c>
-      <c r="D12" s="80" t="s">
+      <c r="D12" s="87" t="s">
         <v>193</v>
       </c>
       <c r="E12" s="47">
@@ -37301,7 +37322,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="78">
+      <c r="A13" s="85">
         <v>9.0</v>
       </c>
       <c r="B13" s="51" t="s">
@@ -37310,7 +37331,7 @@
       <c r="C13" s="47">
         <v>21.0</v>
       </c>
-      <c r="D13" s="80" t="s">
+      <c r="D13" s="87" t="s">
         <v>193</v>
       </c>
       <c r="E13" s="47">
@@ -37319,7 +37340,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="78">
+      <c r="A14" s="85">
         <v>10.0</v>
       </c>
       <c r="B14" s="51" t="s">
@@ -37328,7 +37349,7 @@
       <c r="C14" s="47">
         <v>8.0</v>
       </c>
-      <c r="D14" s="80" t="s">
+      <c r="D14" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E14" s="47">
@@ -37337,7 +37358,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="78">
+      <c r="A15" s="85">
         <v>11.0</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -37346,7 +37367,7 @@
       <c r="C15" s="47">
         <v>5.0</v>
       </c>
-      <c r="D15" s="80" t="s">
+      <c r="D15" s="87" t="s">
         <v>185</v>
       </c>
       <c r="E15" s="47">
@@ -37355,7 +37376,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="78">
+      <c r="A16" s="85">
         <v>12.0</v>
       </c>
       <c r="B16" s="51" t="s">
@@ -37364,7 +37385,7 @@
       <c r="C16" s="47">
         <v>13.0</v>
       </c>
-      <c r="D16" s="80" t="s">
+      <c r="D16" s="87" t="s">
         <v>190</v>
       </c>
       <c r="E16" s="47">
@@ -37373,7 +37394,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="78">
+      <c r="A17" s="85">
         <v>13.0</v>
       </c>
       <c r="B17" s="51" t="s">
@@ -37382,7 +37403,7 @@
       <c r="C17" s="47">
         <v>8.0</v>
       </c>
-      <c r="D17" s="80" t="s">
+      <c r="D17" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E17" s="47">
@@ -37391,16 +37412,16 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="78">
+      <c r="A18" s="85">
         <v>14.0</v>
       </c>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="88" t="s">
         <v>199</v>
       </c>
       <c r="C18" s="47">
         <v>8.0</v>
       </c>
-      <c r="D18" s="80" t="s">
+      <c r="D18" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E18" s="47">
@@ -37409,7 +37430,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="78">
+      <c r="A19" s="85">
         <v>15.0</v>
       </c>
       <c r="B19" s="51" t="s">
@@ -37418,7 +37439,7 @@
       <c r="C19" s="47">
         <v>8.0</v>
       </c>
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E19" s="47">
@@ -37427,7 +37448,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="78">
+      <c r="A20" s="85">
         <v>16.0</v>
       </c>
       <c r="B20" s="51" t="s">
@@ -37436,15 +37457,15 @@
       <c r="C20" s="47">
         <v>3.0</v>
       </c>
-      <c r="D20" s="80" t="s">
+      <c r="D20" s="87" t="s">
         <v>202</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="86">
         <v>6.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="78">
+      <c r="A21" s="85">
         <v>17.0</v>
       </c>
       <c r="B21" s="51" t="s">
@@ -37453,15 +37474,15 @@
       <c r="C21" s="47">
         <v>3.0</v>
       </c>
-      <c r="D21" s="80" t="s">
+      <c r="D21" s="87" t="s">
         <v>204</v>
       </c>
-      <c r="E21" s="79">
+      <c r="E21" s="86">
         <v>6.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="78">
+      <c r="A22" s="85">
         <v>18.0</v>
       </c>
       <c r="B22" s="51" t="s">
@@ -37470,15 +37491,15 @@
       <c r="C22" s="47">
         <v>3.0</v>
       </c>
-      <c r="D22" s="80" t="s">
+      <c r="D22" s="87" t="s">
         <v>204</v>
       </c>
-      <c r="E22" s="79">
+      <c r="E22" s="86">
         <v>6.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="78">
+      <c r="A23" s="85">
         <v>19.0</v>
       </c>
       <c r="B23" s="51" t="s">
@@ -37487,15 +37508,15 @@
       <c r="C23" s="47">
         <v>3.0</v>
       </c>
-      <c r="D23" s="80" t="s">
+      <c r="D23" s="87" t="s">
         <v>204</v>
       </c>
-      <c r="E23" s="79">
+      <c r="E23" s="86">
         <v>6.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="78">
+      <c r="A24" s="85">
         <v>20.0</v>
       </c>
       <c r="B24" s="51" t="s">
@@ -37504,7 +37525,7 @@
       <c r="C24" s="47">
         <v>5.0</v>
       </c>
-      <c r="D24" s="80" t="s">
+      <c r="D24" s="87" t="s">
         <v>185</v>
       </c>
       <c r="E24" s="47">
@@ -37513,16 +37534,16 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="78">
+      <c r="A25" s="85">
         <v>21.0</v>
       </c>
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="88" t="s">
         <v>208</v>
       </c>
-      <c r="C25" s="79">
+      <c r="C25" s="86">
         <v>8.0</v>
       </c>
-      <c r="D25" s="80" t="s">
+      <c r="D25" s="87" t="s">
         <v>209</v>
       </c>
       <c r="E25" s="47">
@@ -37531,7 +37552,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="78">
+      <c r="A26" s="85">
         <v>22.0</v>
       </c>
       <c r="B26" s="51" t="s">
@@ -37540,7 +37561,7 @@
       <c r="C26" s="47">
         <v>8.0</v>
       </c>
-      <c r="D26" s="80" t="s">
+      <c r="D26" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E26" s="47">
@@ -37549,7 +37570,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="78">
+      <c r="A27" s="85">
         <v>23.0</v>
       </c>
       <c r="B27" s="51" t="s">
@@ -37558,7 +37579,7 @@
       <c r="C27" s="47">
         <v>13.0</v>
       </c>
-      <c r="D27" s="80" t="s">
+      <c r="D27" s="87" t="s">
         <v>190</v>
       </c>
       <c r="E27" s="47">
@@ -37567,2926 +37588,2926 @@
       </c>
     </row>
     <row r="28">
-      <c r="D28" s="72"/>
+      <c r="D28" s="79"/>
     </row>
     <row r="29">
-      <c r="D29" s="72"/>
+      <c r="D29" s="79"/>
     </row>
     <row r="30">
-      <c r="D30" s="72"/>
+      <c r="D30" s="79"/>
     </row>
     <row r="31">
-      <c r="D31" s="72"/>
+      <c r="D31" s="79"/>
     </row>
     <row r="32">
-      <c r="D32" s="72"/>
+      <c r="D32" s="79"/>
     </row>
     <row r="33">
-      <c r="D33" s="72"/>
+      <c r="D33" s="79"/>
     </row>
     <row r="34">
-      <c r="D34" s="72"/>
+      <c r="D34" s="79"/>
     </row>
     <row r="35">
-      <c r="D35" s="72"/>
+      <c r="D35" s="79"/>
     </row>
     <row r="36">
-      <c r="D36" s="72"/>
+      <c r="D36" s="79"/>
     </row>
     <row r="37">
-      <c r="D37" s="72"/>
+      <c r="D37" s="79"/>
     </row>
     <row r="38">
-      <c r="D38" s="72"/>
+      <c r="D38" s="79"/>
     </row>
     <row r="39">
-      <c r="D39" s="72"/>
+      <c r="D39" s="79"/>
     </row>
     <row r="40">
-      <c r="D40" s="72"/>
+      <c r="D40" s="79"/>
     </row>
     <row r="41">
-      <c r="D41" s="72"/>
+      <c r="D41" s="79"/>
     </row>
     <row r="42">
-      <c r="D42" s="72"/>
+      <c r="D42" s="79"/>
     </row>
     <row r="43">
-      <c r="D43" s="72"/>
+      <c r="D43" s="79"/>
     </row>
     <row r="44">
-      <c r="D44" s="72"/>
+      <c r="D44" s="79"/>
     </row>
     <row r="45">
-      <c r="D45" s="72"/>
+      <c r="D45" s="79"/>
     </row>
     <row r="46">
-      <c r="D46" s="72"/>
+      <c r="D46" s="79"/>
     </row>
     <row r="47">
-      <c r="D47" s="72"/>
+      <c r="D47" s="79"/>
     </row>
     <row r="48">
-      <c r="D48" s="72"/>
+      <c r="D48" s="79"/>
     </row>
     <row r="49">
-      <c r="D49" s="72"/>
+      <c r="D49" s="79"/>
     </row>
     <row r="50">
-      <c r="D50" s="72"/>
+      <c r="D50" s="79"/>
     </row>
     <row r="51">
-      <c r="D51" s="72"/>
+      <c r="D51" s="79"/>
     </row>
     <row r="52">
-      <c r="D52" s="72"/>
+      <c r="D52" s="79"/>
     </row>
     <row r="53">
-      <c r="D53" s="72"/>
+      <c r="D53" s="79"/>
     </row>
     <row r="54">
-      <c r="D54" s="72"/>
+      <c r="D54" s="79"/>
     </row>
     <row r="55">
-      <c r="D55" s="72"/>
+      <c r="D55" s="79"/>
     </row>
     <row r="56">
-      <c r="D56" s="72"/>
+      <c r="D56" s="79"/>
     </row>
     <row r="57">
-      <c r="D57" s="72"/>
+      <c r="D57" s="79"/>
     </row>
     <row r="58">
-      <c r="D58" s="72"/>
+      <c r="D58" s="79"/>
     </row>
     <row r="59">
-      <c r="D59" s="72"/>
+      <c r="D59" s="79"/>
     </row>
     <row r="60">
-      <c r="D60" s="72"/>
+      <c r="D60" s="79"/>
     </row>
     <row r="61">
-      <c r="D61" s="72"/>
+      <c r="D61" s="79"/>
     </row>
     <row r="62">
-      <c r="D62" s="72"/>
+      <c r="D62" s="79"/>
     </row>
     <row r="63">
-      <c r="D63" s="72"/>
+      <c r="D63" s="79"/>
     </row>
     <row r="64">
-      <c r="D64" s="72"/>
+      <c r="D64" s="79"/>
     </row>
     <row r="65">
-      <c r="D65" s="72"/>
+      <c r="D65" s="79"/>
     </row>
     <row r="66">
-      <c r="D66" s="72"/>
+      <c r="D66" s="79"/>
     </row>
     <row r="67">
-      <c r="D67" s="72"/>
+      <c r="D67" s="79"/>
     </row>
     <row r="68">
-      <c r="D68" s="72"/>
+      <c r="D68" s="79"/>
     </row>
     <row r="69">
-      <c r="D69" s="72"/>
+      <c r="D69" s="79"/>
     </row>
     <row r="70">
-      <c r="D70" s="72"/>
+      <c r="D70" s="79"/>
     </row>
     <row r="71">
-      <c r="D71" s="72"/>
+      <c r="D71" s="79"/>
     </row>
     <row r="72">
-      <c r="D72" s="72"/>
+      <c r="D72" s="79"/>
     </row>
     <row r="73">
-      <c r="D73" s="72"/>
+      <c r="D73" s="79"/>
     </row>
     <row r="74">
-      <c r="D74" s="72"/>
+      <c r="D74" s="79"/>
     </row>
     <row r="75">
-      <c r="D75" s="72"/>
+      <c r="D75" s="79"/>
     </row>
     <row r="76">
-      <c r="D76" s="72"/>
+      <c r="D76" s="79"/>
     </row>
     <row r="77">
-      <c r="D77" s="72"/>
+      <c r="D77" s="79"/>
     </row>
     <row r="78">
-      <c r="D78" s="72"/>
+      <c r="D78" s="79"/>
     </row>
     <row r="79">
-      <c r="D79" s="72"/>
+      <c r="D79" s="79"/>
     </row>
     <row r="80">
-      <c r="D80" s="72"/>
+      <c r="D80" s="79"/>
     </row>
     <row r="81">
-      <c r="D81" s="72"/>
+      <c r="D81" s="79"/>
     </row>
     <row r="82">
-      <c r="D82" s="72"/>
+      <c r="D82" s="79"/>
     </row>
     <row r="83">
-      <c r="D83" s="72"/>
+      <c r="D83" s="79"/>
     </row>
     <row r="84">
-      <c r="D84" s="72"/>
+      <c r="D84" s="79"/>
     </row>
     <row r="85">
-      <c r="D85" s="72"/>
+      <c r="D85" s="79"/>
     </row>
     <row r="86">
-      <c r="D86" s="72"/>
+      <c r="D86" s="79"/>
     </row>
     <row r="87">
-      <c r="D87" s="72"/>
+      <c r="D87" s="79"/>
     </row>
     <row r="88">
-      <c r="D88" s="72"/>
+      <c r="D88" s="79"/>
     </row>
     <row r="89">
-      <c r="D89" s="72"/>
+      <c r="D89" s="79"/>
     </row>
     <row r="90">
-      <c r="D90" s="72"/>
+      <c r="D90" s="79"/>
     </row>
     <row r="91">
-      <c r="D91" s="72"/>
+      <c r="D91" s="79"/>
     </row>
     <row r="92">
-      <c r="D92" s="72"/>
+      <c r="D92" s="79"/>
     </row>
     <row r="93">
-      <c r="D93" s="72"/>
+      <c r="D93" s="79"/>
     </row>
     <row r="94">
-      <c r="D94" s="72"/>
+      <c r="D94" s="79"/>
     </row>
     <row r="95">
-      <c r="D95" s="72"/>
+      <c r="D95" s="79"/>
     </row>
     <row r="96">
-      <c r="D96" s="72"/>
+      <c r="D96" s="79"/>
     </row>
     <row r="97">
-      <c r="D97" s="72"/>
+      <c r="D97" s="79"/>
     </row>
     <row r="98">
-      <c r="D98" s="72"/>
+      <c r="D98" s="79"/>
     </row>
     <row r="99">
-      <c r="D99" s="72"/>
+      <c r="D99" s="79"/>
     </row>
     <row r="100">
-      <c r="D100" s="72"/>
+      <c r="D100" s="79"/>
     </row>
     <row r="101">
-      <c r="D101" s="72"/>
+      <c r="D101" s="79"/>
     </row>
     <row r="102">
-      <c r="D102" s="72"/>
+      <c r="D102" s="79"/>
     </row>
     <row r="103">
-      <c r="D103" s="72"/>
+      <c r="D103" s="79"/>
     </row>
     <row r="104">
-      <c r="D104" s="72"/>
+      <c r="D104" s="79"/>
     </row>
     <row r="105">
-      <c r="D105" s="72"/>
+      <c r="D105" s="79"/>
     </row>
     <row r="106">
-      <c r="D106" s="72"/>
+      <c r="D106" s="79"/>
     </row>
     <row r="107">
-      <c r="D107" s="72"/>
+      <c r="D107" s="79"/>
     </row>
     <row r="108">
-      <c r="D108" s="72"/>
+      <c r="D108" s="79"/>
     </row>
     <row r="109">
-      <c r="D109" s="72"/>
+      <c r="D109" s="79"/>
     </row>
     <row r="110">
-      <c r="D110" s="72"/>
+      <c r="D110" s="79"/>
     </row>
     <row r="111">
-      <c r="D111" s="72"/>
+      <c r="D111" s="79"/>
     </row>
     <row r="112">
-      <c r="D112" s="72"/>
+      <c r="D112" s="79"/>
     </row>
     <row r="113">
-      <c r="D113" s="72"/>
+      <c r="D113" s="79"/>
     </row>
     <row r="114">
-      <c r="D114" s="72"/>
+      <c r="D114" s="79"/>
     </row>
     <row r="115">
-      <c r="D115" s="72"/>
+      <c r="D115" s="79"/>
     </row>
     <row r="116">
-      <c r="D116" s="72"/>
+      <c r="D116" s="79"/>
     </row>
     <row r="117">
-      <c r="D117" s="72"/>
+      <c r="D117" s="79"/>
     </row>
     <row r="118">
-      <c r="D118" s="72"/>
+      <c r="D118" s="79"/>
     </row>
     <row r="119">
-      <c r="D119" s="72"/>
+      <c r="D119" s="79"/>
     </row>
     <row r="120">
-      <c r="D120" s="72"/>
+      <c r="D120" s="79"/>
     </row>
     <row r="121">
-      <c r="D121" s="72"/>
+      <c r="D121" s="79"/>
     </row>
     <row r="122">
-      <c r="D122" s="72"/>
+      <c r="D122" s="79"/>
     </row>
     <row r="123">
-      <c r="D123" s="72"/>
+      <c r="D123" s="79"/>
     </row>
     <row r="124">
-      <c r="D124" s="72"/>
+      <c r="D124" s="79"/>
     </row>
     <row r="125">
-      <c r="D125" s="72"/>
+      <c r="D125" s="79"/>
     </row>
     <row r="126">
-      <c r="D126" s="72"/>
+      <c r="D126" s="79"/>
     </row>
     <row r="127">
-      <c r="D127" s="72"/>
+      <c r="D127" s="79"/>
     </row>
     <row r="128">
-      <c r="D128" s="72"/>
+      <c r="D128" s="79"/>
     </row>
     <row r="129">
-      <c r="D129" s="72"/>
+      <c r="D129" s="79"/>
     </row>
     <row r="130">
-      <c r="D130" s="72"/>
+      <c r="D130" s="79"/>
     </row>
     <row r="131">
-      <c r="D131" s="72"/>
+      <c r="D131" s="79"/>
     </row>
     <row r="132">
-      <c r="D132" s="72"/>
+      <c r="D132" s="79"/>
     </row>
     <row r="133">
-      <c r="D133" s="72"/>
+      <c r="D133" s="79"/>
     </row>
     <row r="134">
-      <c r="D134" s="72"/>
+      <c r="D134" s="79"/>
     </row>
     <row r="135">
-      <c r="D135" s="72"/>
+      <c r="D135" s="79"/>
     </row>
     <row r="136">
-      <c r="D136" s="72"/>
+      <c r="D136" s="79"/>
     </row>
     <row r="137">
-      <c r="D137" s="72"/>
+      <c r="D137" s="79"/>
     </row>
     <row r="138">
-      <c r="D138" s="72"/>
+      <c r="D138" s="79"/>
     </row>
     <row r="139">
-      <c r="D139" s="72"/>
+      <c r="D139" s="79"/>
     </row>
     <row r="140">
-      <c r="D140" s="72"/>
+      <c r="D140" s="79"/>
     </row>
     <row r="141">
-      <c r="D141" s="72"/>
+      <c r="D141" s="79"/>
     </row>
     <row r="142">
-      <c r="D142" s="72"/>
+      <c r="D142" s="79"/>
     </row>
     <row r="143">
-      <c r="D143" s="72"/>
+      <c r="D143" s="79"/>
     </row>
     <row r="144">
-      <c r="D144" s="72"/>
+      <c r="D144" s="79"/>
     </row>
     <row r="145">
-      <c r="D145" s="72"/>
+      <c r="D145" s="79"/>
     </row>
     <row r="146">
-      <c r="D146" s="72"/>
+      <c r="D146" s="79"/>
     </row>
     <row r="147">
-      <c r="D147" s="72"/>
+      <c r="D147" s="79"/>
     </row>
     <row r="148">
-      <c r="D148" s="72"/>
+      <c r="D148" s="79"/>
     </row>
     <row r="149">
-      <c r="D149" s="72"/>
+      <c r="D149" s="79"/>
     </row>
     <row r="150">
-      <c r="D150" s="72"/>
+      <c r="D150" s="79"/>
     </row>
     <row r="151">
-      <c r="D151" s="72"/>
+      <c r="D151" s="79"/>
     </row>
     <row r="152">
-      <c r="D152" s="72"/>
+      <c r="D152" s="79"/>
     </row>
     <row r="153">
-      <c r="D153" s="72"/>
+      <c r="D153" s="79"/>
     </row>
     <row r="154">
-      <c r="D154" s="72"/>
+      <c r="D154" s="79"/>
     </row>
     <row r="155">
-      <c r="D155" s="72"/>
+      <c r="D155" s="79"/>
     </row>
     <row r="156">
-      <c r="D156" s="72"/>
+      <c r="D156" s="79"/>
     </row>
     <row r="157">
-      <c r="D157" s="72"/>
+      <c r="D157" s="79"/>
     </row>
     <row r="158">
-      <c r="D158" s="72"/>
+      <c r="D158" s="79"/>
     </row>
     <row r="159">
-      <c r="D159" s="72"/>
+      <c r="D159" s="79"/>
     </row>
     <row r="160">
-      <c r="D160" s="72"/>
+      <c r="D160" s="79"/>
     </row>
     <row r="161">
-      <c r="D161" s="72"/>
+      <c r="D161" s="79"/>
     </row>
     <row r="162">
-      <c r="D162" s="72"/>
+      <c r="D162" s="79"/>
     </row>
     <row r="163">
-      <c r="D163" s="72"/>
+      <c r="D163" s="79"/>
     </row>
     <row r="164">
-      <c r="D164" s="72"/>
+      <c r="D164" s="79"/>
     </row>
     <row r="165">
-      <c r="D165" s="72"/>
+      <c r="D165" s="79"/>
     </row>
     <row r="166">
-      <c r="D166" s="72"/>
+      <c r="D166" s="79"/>
     </row>
     <row r="167">
-      <c r="D167" s="72"/>
+      <c r="D167" s="79"/>
     </row>
     <row r="168">
-      <c r="D168" s="72"/>
+      <c r="D168" s="79"/>
     </row>
     <row r="169">
-      <c r="D169" s="72"/>
+      <c r="D169" s="79"/>
     </row>
     <row r="170">
-      <c r="D170" s="72"/>
+      <c r="D170" s="79"/>
     </row>
     <row r="171">
-      <c r="D171" s="72"/>
+      <c r="D171" s="79"/>
     </row>
     <row r="172">
-      <c r="D172" s="72"/>
+      <c r="D172" s="79"/>
     </row>
     <row r="173">
-      <c r="D173" s="72"/>
+      <c r="D173" s="79"/>
     </row>
     <row r="174">
-      <c r="D174" s="72"/>
+      <c r="D174" s="79"/>
     </row>
     <row r="175">
-      <c r="D175" s="72"/>
+      <c r="D175" s="79"/>
     </row>
     <row r="176">
-      <c r="D176" s="72"/>
+      <c r="D176" s="79"/>
     </row>
     <row r="177">
-      <c r="D177" s="72"/>
+      <c r="D177" s="79"/>
     </row>
     <row r="178">
-      <c r="D178" s="72"/>
+      <c r="D178" s="79"/>
     </row>
     <row r="179">
-      <c r="D179" s="72"/>
+      <c r="D179" s="79"/>
     </row>
     <row r="180">
-      <c r="D180" s="72"/>
+      <c r="D180" s="79"/>
     </row>
     <row r="181">
-      <c r="D181" s="72"/>
+      <c r="D181" s="79"/>
     </row>
     <row r="182">
-      <c r="D182" s="72"/>
+      <c r="D182" s="79"/>
     </row>
     <row r="183">
-      <c r="D183" s="72"/>
+      <c r="D183" s="79"/>
     </row>
     <row r="184">
-      <c r="D184" s="72"/>
+      <c r="D184" s="79"/>
     </row>
     <row r="185">
-      <c r="D185" s="72"/>
+      <c r="D185" s="79"/>
     </row>
     <row r="186">
-      <c r="D186" s="72"/>
+      <c r="D186" s="79"/>
     </row>
     <row r="187">
-      <c r="D187" s="72"/>
+      <c r="D187" s="79"/>
     </row>
     <row r="188">
-      <c r="D188" s="72"/>
+      <c r="D188" s="79"/>
     </row>
     <row r="189">
-      <c r="D189" s="72"/>
+      <c r="D189" s="79"/>
     </row>
     <row r="190">
-      <c r="D190" s="72"/>
+      <c r="D190" s="79"/>
     </row>
     <row r="191">
-      <c r="D191" s="72"/>
+      <c r="D191" s="79"/>
     </row>
     <row r="192">
-      <c r="D192" s="72"/>
+      <c r="D192" s="79"/>
     </row>
     <row r="193">
-      <c r="D193" s="72"/>
+      <c r="D193" s="79"/>
     </row>
     <row r="194">
-      <c r="D194" s="72"/>
+      <c r="D194" s="79"/>
     </row>
     <row r="195">
-      <c r="D195" s="72"/>
+      <c r="D195" s="79"/>
     </row>
     <row r="196">
-      <c r="D196" s="72"/>
+      <c r="D196" s="79"/>
     </row>
     <row r="197">
-      <c r="D197" s="72"/>
+      <c r="D197" s="79"/>
     </row>
     <row r="198">
-      <c r="D198" s="72"/>
+      <c r="D198" s="79"/>
     </row>
     <row r="199">
-      <c r="D199" s="72"/>
+      <c r="D199" s="79"/>
     </row>
     <row r="200">
-      <c r="D200" s="72"/>
+      <c r="D200" s="79"/>
     </row>
     <row r="201">
-      <c r="D201" s="72"/>
+      <c r="D201" s="79"/>
     </row>
     <row r="202">
-      <c r="D202" s="72"/>
+      <c r="D202" s="79"/>
     </row>
     <row r="203">
-      <c r="D203" s="72"/>
+      <c r="D203" s="79"/>
     </row>
     <row r="204">
-      <c r="D204" s="72"/>
+      <c r="D204" s="79"/>
     </row>
     <row r="205">
-      <c r="D205" s="72"/>
+      <c r="D205" s="79"/>
     </row>
     <row r="206">
-      <c r="D206" s="72"/>
+      <c r="D206" s="79"/>
     </row>
     <row r="207">
-      <c r="D207" s="72"/>
+      <c r="D207" s="79"/>
     </row>
     <row r="208">
-      <c r="D208" s="72"/>
+      <c r="D208" s="79"/>
     </row>
     <row r="209">
-      <c r="D209" s="72"/>
+      <c r="D209" s="79"/>
     </row>
     <row r="210">
-      <c r="D210" s="72"/>
+      <c r="D210" s="79"/>
     </row>
     <row r="211">
-      <c r="D211" s="72"/>
+      <c r="D211" s="79"/>
     </row>
     <row r="212">
-      <c r="D212" s="72"/>
+      <c r="D212" s="79"/>
     </row>
     <row r="213">
-      <c r="D213" s="72"/>
+      <c r="D213" s="79"/>
     </row>
     <row r="214">
-      <c r="D214" s="72"/>
+      <c r="D214" s="79"/>
     </row>
     <row r="215">
-      <c r="D215" s="72"/>
+      <c r="D215" s="79"/>
     </row>
     <row r="216">
-      <c r="D216" s="72"/>
+      <c r="D216" s="79"/>
     </row>
     <row r="217">
-      <c r="D217" s="72"/>
+      <c r="D217" s="79"/>
     </row>
     <row r="218">
-      <c r="D218" s="72"/>
+      <c r="D218" s="79"/>
     </row>
     <row r="219">
-      <c r="D219" s="72"/>
+      <c r="D219" s="79"/>
     </row>
     <row r="220">
-      <c r="D220" s="72"/>
+      <c r="D220" s="79"/>
     </row>
     <row r="221">
-      <c r="D221" s="72"/>
+      <c r="D221" s="79"/>
     </row>
     <row r="222">
-      <c r="D222" s="72"/>
+      <c r="D222" s="79"/>
     </row>
     <row r="223">
-      <c r="D223" s="72"/>
+      <c r="D223" s="79"/>
     </row>
     <row r="224">
-      <c r="D224" s="72"/>
+      <c r="D224" s="79"/>
     </row>
     <row r="225">
-      <c r="D225" s="72"/>
+      <c r="D225" s="79"/>
     </row>
     <row r="226">
-      <c r="D226" s="72"/>
+      <c r="D226" s="79"/>
     </row>
     <row r="227">
-      <c r="D227" s="72"/>
+      <c r="D227" s="79"/>
     </row>
     <row r="228">
-      <c r="D228" s="72"/>
+      <c r="D228" s="79"/>
     </row>
     <row r="229">
-      <c r="D229" s="72"/>
+      <c r="D229" s="79"/>
     </row>
     <row r="230">
-      <c r="D230" s="72"/>
+      <c r="D230" s="79"/>
     </row>
     <row r="231">
-      <c r="D231" s="72"/>
+      <c r="D231" s="79"/>
     </row>
     <row r="232">
-      <c r="D232" s="72"/>
+      <c r="D232" s="79"/>
     </row>
     <row r="233">
-      <c r="D233" s="72"/>
+      <c r="D233" s="79"/>
     </row>
     <row r="234">
-      <c r="D234" s="72"/>
+      <c r="D234" s="79"/>
     </row>
     <row r="235">
-      <c r="D235" s="72"/>
+      <c r="D235" s="79"/>
     </row>
     <row r="236">
-      <c r="D236" s="72"/>
+      <c r="D236" s="79"/>
     </row>
     <row r="237">
-      <c r="D237" s="72"/>
+      <c r="D237" s="79"/>
     </row>
     <row r="238">
-      <c r="D238" s="72"/>
+      <c r="D238" s="79"/>
     </row>
     <row r="239">
-      <c r="D239" s="72"/>
+      <c r="D239" s="79"/>
     </row>
     <row r="240">
-      <c r="D240" s="72"/>
+      <c r="D240" s="79"/>
     </row>
     <row r="241">
-      <c r="D241" s="72"/>
+      <c r="D241" s="79"/>
     </row>
     <row r="242">
-      <c r="D242" s="72"/>
+      <c r="D242" s="79"/>
     </row>
     <row r="243">
-      <c r="D243" s="72"/>
+      <c r="D243" s="79"/>
     </row>
     <row r="244">
-      <c r="D244" s="72"/>
+      <c r="D244" s="79"/>
     </row>
     <row r="245">
-      <c r="D245" s="72"/>
+      <c r="D245" s="79"/>
     </row>
     <row r="246">
-      <c r="D246" s="72"/>
+      <c r="D246" s="79"/>
     </row>
     <row r="247">
-      <c r="D247" s="72"/>
+      <c r="D247" s="79"/>
     </row>
     <row r="248">
-      <c r="D248" s="72"/>
+      <c r="D248" s="79"/>
     </row>
     <row r="249">
-      <c r="D249" s="72"/>
+      <c r="D249" s="79"/>
     </row>
     <row r="250">
-      <c r="D250" s="72"/>
+      <c r="D250" s="79"/>
     </row>
     <row r="251">
-      <c r="D251" s="72"/>
+      <c r="D251" s="79"/>
     </row>
     <row r="252">
-      <c r="D252" s="72"/>
+      <c r="D252" s="79"/>
     </row>
     <row r="253">
-      <c r="D253" s="72"/>
+      <c r="D253" s="79"/>
     </row>
     <row r="254">
-      <c r="D254" s="72"/>
+      <c r="D254" s="79"/>
     </row>
     <row r="255">
-      <c r="D255" s="72"/>
+      <c r="D255" s="79"/>
     </row>
     <row r="256">
-      <c r="D256" s="72"/>
+      <c r="D256" s="79"/>
     </row>
     <row r="257">
-      <c r="D257" s="72"/>
+      <c r="D257" s="79"/>
     </row>
     <row r="258">
-      <c r="D258" s="72"/>
+      <c r="D258" s="79"/>
     </row>
     <row r="259">
-      <c r="D259" s="72"/>
+      <c r="D259" s="79"/>
     </row>
     <row r="260">
-      <c r="D260" s="72"/>
+      <c r="D260" s="79"/>
     </row>
     <row r="261">
-      <c r="D261" s="72"/>
+      <c r="D261" s="79"/>
     </row>
     <row r="262">
-      <c r="D262" s="72"/>
+      <c r="D262" s="79"/>
     </row>
     <row r="263">
-      <c r="D263" s="72"/>
+      <c r="D263" s="79"/>
     </row>
     <row r="264">
-      <c r="D264" s="72"/>
+      <c r="D264" s="79"/>
     </row>
     <row r="265">
-      <c r="D265" s="72"/>
+      <c r="D265" s="79"/>
     </row>
     <row r="266">
-      <c r="D266" s="72"/>
+      <c r="D266" s="79"/>
     </row>
     <row r="267">
-      <c r="D267" s="72"/>
+      <c r="D267" s="79"/>
     </row>
     <row r="268">
-      <c r="D268" s="72"/>
+      <c r="D268" s="79"/>
     </row>
     <row r="269">
-      <c r="D269" s="72"/>
+      <c r="D269" s="79"/>
     </row>
     <row r="270">
-      <c r="D270" s="72"/>
+      <c r="D270" s="79"/>
     </row>
     <row r="271">
-      <c r="D271" s="72"/>
+      <c r="D271" s="79"/>
     </row>
     <row r="272">
-      <c r="D272" s="72"/>
+      <c r="D272" s="79"/>
     </row>
     <row r="273">
-      <c r="D273" s="72"/>
+      <c r="D273" s="79"/>
     </row>
     <row r="274">
-      <c r="D274" s="72"/>
+      <c r="D274" s="79"/>
     </row>
     <row r="275">
-      <c r="D275" s="72"/>
+      <c r="D275" s="79"/>
     </row>
     <row r="276">
-      <c r="D276" s="72"/>
+      <c r="D276" s="79"/>
     </row>
     <row r="277">
-      <c r="D277" s="72"/>
+      <c r="D277" s="79"/>
     </row>
     <row r="278">
-      <c r="D278" s="72"/>
+      <c r="D278" s="79"/>
     </row>
     <row r="279">
-      <c r="D279" s="72"/>
+      <c r="D279" s="79"/>
     </row>
     <row r="280">
-      <c r="D280" s="72"/>
+      <c r="D280" s="79"/>
     </row>
     <row r="281">
-      <c r="D281" s="72"/>
+      <c r="D281" s="79"/>
     </row>
     <row r="282">
-      <c r="D282" s="72"/>
+      <c r="D282" s="79"/>
     </row>
     <row r="283">
-      <c r="D283" s="72"/>
+      <c r="D283" s="79"/>
     </row>
     <row r="284">
-      <c r="D284" s="72"/>
+      <c r="D284" s="79"/>
     </row>
     <row r="285">
-      <c r="D285" s="72"/>
+      <c r="D285" s="79"/>
     </row>
     <row r="286">
-      <c r="D286" s="72"/>
+      <c r="D286" s="79"/>
     </row>
     <row r="287">
-      <c r="D287" s="72"/>
+      <c r="D287" s="79"/>
     </row>
     <row r="288">
-      <c r="D288" s="72"/>
+      <c r="D288" s="79"/>
     </row>
     <row r="289">
-      <c r="D289" s="72"/>
+      <c r="D289" s="79"/>
     </row>
     <row r="290">
-      <c r="D290" s="72"/>
+      <c r="D290" s="79"/>
     </row>
     <row r="291">
-      <c r="D291" s="72"/>
+      <c r="D291" s="79"/>
     </row>
     <row r="292">
-      <c r="D292" s="72"/>
+      <c r="D292" s="79"/>
     </row>
     <row r="293">
-      <c r="D293" s="72"/>
+      <c r="D293" s="79"/>
     </row>
     <row r="294">
-      <c r="D294" s="72"/>
+      <c r="D294" s="79"/>
     </row>
     <row r="295">
-      <c r="D295" s="72"/>
+      <c r="D295" s="79"/>
     </row>
     <row r="296">
-      <c r="D296" s="72"/>
+      <c r="D296" s="79"/>
     </row>
     <row r="297">
-      <c r="D297" s="72"/>
+      <c r="D297" s="79"/>
     </row>
     <row r="298">
-      <c r="D298" s="72"/>
+      <c r="D298" s="79"/>
     </row>
     <row r="299">
-      <c r="D299" s="72"/>
+      <c r="D299" s="79"/>
     </row>
     <row r="300">
-      <c r="D300" s="72"/>
+      <c r="D300" s="79"/>
     </row>
     <row r="301">
-      <c r="D301" s="72"/>
+      <c r="D301" s="79"/>
     </row>
     <row r="302">
-      <c r="D302" s="72"/>
+      <c r="D302" s="79"/>
     </row>
     <row r="303">
-      <c r="D303" s="72"/>
+      <c r="D303" s="79"/>
     </row>
     <row r="304">
-      <c r="D304" s="72"/>
+      <c r="D304" s="79"/>
     </row>
     <row r="305">
-      <c r="D305" s="72"/>
+      <c r="D305" s="79"/>
     </row>
     <row r="306">
-      <c r="D306" s="72"/>
+      <c r="D306" s="79"/>
     </row>
     <row r="307">
-      <c r="D307" s="72"/>
+      <c r="D307" s="79"/>
     </row>
     <row r="308">
-      <c r="D308" s="72"/>
+      <c r="D308" s="79"/>
     </row>
     <row r="309">
-      <c r="D309" s="72"/>
+      <c r="D309" s="79"/>
     </row>
     <row r="310">
-      <c r="D310" s="72"/>
+      <c r="D310" s="79"/>
     </row>
     <row r="311">
-      <c r="D311" s="72"/>
+      <c r="D311" s="79"/>
     </row>
     <row r="312">
-      <c r="D312" s="72"/>
+      <c r="D312" s="79"/>
     </row>
     <row r="313">
-      <c r="D313" s="72"/>
+      <c r="D313" s="79"/>
     </row>
     <row r="314">
-      <c r="D314" s="72"/>
+      <c r="D314" s="79"/>
     </row>
     <row r="315">
-      <c r="D315" s="72"/>
+      <c r="D315" s="79"/>
     </row>
     <row r="316">
-      <c r="D316" s="72"/>
+      <c r="D316" s="79"/>
     </row>
     <row r="317">
-      <c r="D317" s="72"/>
+      <c r="D317" s="79"/>
     </row>
     <row r="318">
-      <c r="D318" s="72"/>
+      <c r="D318" s="79"/>
     </row>
     <row r="319">
-      <c r="D319" s="72"/>
+      <c r="D319" s="79"/>
     </row>
     <row r="320">
-      <c r="D320" s="72"/>
+      <c r="D320" s="79"/>
     </row>
     <row r="321">
-      <c r="D321" s="72"/>
+      <c r="D321" s="79"/>
     </row>
     <row r="322">
-      <c r="D322" s="72"/>
+      <c r="D322" s="79"/>
     </row>
     <row r="323">
-      <c r="D323" s="72"/>
+      <c r="D323" s="79"/>
     </row>
     <row r="324">
-      <c r="D324" s="72"/>
+      <c r="D324" s="79"/>
     </row>
     <row r="325">
-      <c r="D325" s="72"/>
+      <c r="D325" s="79"/>
     </row>
     <row r="326">
-      <c r="D326" s="72"/>
+      <c r="D326" s="79"/>
     </row>
     <row r="327">
-      <c r="D327" s="72"/>
+      <c r="D327" s="79"/>
     </row>
     <row r="328">
-      <c r="D328" s="72"/>
+      <c r="D328" s="79"/>
     </row>
     <row r="329">
-      <c r="D329" s="72"/>
+      <c r="D329" s="79"/>
     </row>
     <row r="330">
-      <c r="D330" s="72"/>
+      <c r="D330" s="79"/>
     </row>
     <row r="331">
-      <c r="D331" s="72"/>
+      <c r="D331" s="79"/>
     </row>
     <row r="332">
-      <c r="D332" s="72"/>
+      <c r="D332" s="79"/>
     </row>
     <row r="333">
-      <c r="D333" s="72"/>
+      <c r="D333" s="79"/>
     </row>
     <row r="334">
-      <c r="D334" s="72"/>
+      <c r="D334" s="79"/>
     </row>
     <row r="335">
-      <c r="D335" s="72"/>
+      <c r="D335" s="79"/>
     </row>
     <row r="336">
-      <c r="D336" s="72"/>
+      <c r="D336" s="79"/>
     </row>
     <row r="337">
-      <c r="D337" s="72"/>
+      <c r="D337" s="79"/>
     </row>
     <row r="338">
-      <c r="D338" s="72"/>
+      <c r="D338" s="79"/>
     </row>
     <row r="339">
-      <c r="D339" s="72"/>
+      <c r="D339" s="79"/>
     </row>
     <row r="340">
-      <c r="D340" s="72"/>
+      <c r="D340" s="79"/>
     </row>
     <row r="341">
-      <c r="D341" s="72"/>
+      <c r="D341" s="79"/>
     </row>
     <row r="342">
-      <c r="D342" s="72"/>
+      <c r="D342" s="79"/>
     </row>
     <row r="343">
-      <c r="D343" s="72"/>
+      <c r="D343" s="79"/>
     </row>
     <row r="344">
-      <c r="D344" s="72"/>
+      <c r="D344" s="79"/>
     </row>
     <row r="345">
-      <c r="D345" s="72"/>
+      <c r="D345" s="79"/>
     </row>
     <row r="346">
-      <c r="D346" s="72"/>
+      <c r="D346" s="79"/>
     </row>
     <row r="347">
-      <c r="D347" s="72"/>
+      <c r="D347" s="79"/>
     </row>
     <row r="348">
-      <c r="D348" s="72"/>
+      <c r="D348" s="79"/>
     </row>
     <row r="349">
-      <c r="D349" s="72"/>
+      <c r="D349" s="79"/>
     </row>
     <row r="350">
-      <c r="D350" s="72"/>
+      <c r="D350" s="79"/>
     </row>
     <row r="351">
-      <c r="D351" s="72"/>
+      <c r="D351" s="79"/>
     </row>
     <row r="352">
-      <c r="D352" s="72"/>
+      <c r="D352" s="79"/>
     </row>
     <row r="353">
-      <c r="D353" s="72"/>
+      <c r="D353" s="79"/>
     </row>
     <row r="354">
-      <c r="D354" s="72"/>
+      <c r="D354" s="79"/>
     </row>
     <row r="355">
-      <c r="D355" s="72"/>
+      <c r="D355" s="79"/>
     </row>
     <row r="356">
-      <c r="D356" s="72"/>
+      <c r="D356" s="79"/>
     </row>
     <row r="357">
-      <c r="D357" s="72"/>
+      <c r="D357" s="79"/>
     </row>
     <row r="358">
-      <c r="D358" s="72"/>
+      <c r="D358" s="79"/>
     </row>
     <row r="359">
-      <c r="D359" s="72"/>
+      <c r="D359" s="79"/>
     </row>
     <row r="360">
-      <c r="D360" s="72"/>
+      <c r="D360" s="79"/>
     </row>
     <row r="361">
-      <c r="D361" s="72"/>
+      <c r="D361" s="79"/>
     </row>
     <row r="362">
-      <c r="D362" s="72"/>
+      <c r="D362" s="79"/>
     </row>
     <row r="363">
-      <c r="D363" s="72"/>
+      <c r="D363" s="79"/>
     </row>
     <row r="364">
-      <c r="D364" s="72"/>
+      <c r="D364" s="79"/>
     </row>
     <row r="365">
-      <c r="D365" s="72"/>
+      <c r="D365" s="79"/>
     </row>
     <row r="366">
-      <c r="D366" s="72"/>
+      <c r="D366" s="79"/>
     </row>
     <row r="367">
-      <c r="D367" s="72"/>
+      <c r="D367" s="79"/>
     </row>
     <row r="368">
-      <c r="D368" s="72"/>
+      <c r="D368" s="79"/>
     </row>
     <row r="369">
-      <c r="D369" s="72"/>
+      <c r="D369" s="79"/>
     </row>
     <row r="370">
-      <c r="D370" s="72"/>
+      <c r="D370" s="79"/>
     </row>
     <row r="371">
-      <c r="D371" s="72"/>
+      <c r="D371" s="79"/>
     </row>
     <row r="372">
-      <c r="D372" s="72"/>
+      <c r="D372" s="79"/>
     </row>
     <row r="373">
-      <c r="D373" s="72"/>
+      <c r="D373" s="79"/>
     </row>
     <row r="374">
-      <c r="D374" s="72"/>
+      <c r="D374" s="79"/>
     </row>
     <row r="375">
-      <c r="D375" s="72"/>
+      <c r="D375" s="79"/>
     </row>
     <row r="376">
-      <c r="D376" s="72"/>
+      <c r="D376" s="79"/>
     </row>
     <row r="377">
-      <c r="D377" s="72"/>
+      <c r="D377" s="79"/>
     </row>
     <row r="378">
-      <c r="D378" s="72"/>
+      <c r="D378" s="79"/>
     </row>
     <row r="379">
-      <c r="D379" s="72"/>
+      <c r="D379" s="79"/>
     </row>
     <row r="380">
-      <c r="D380" s="72"/>
+      <c r="D380" s="79"/>
     </row>
     <row r="381">
-      <c r="D381" s="72"/>
+      <c r="D381" s="79"/>
     </row>
     <row r="382">
-      <c r="D382" s="72"/>
+      <c r="D382" s="79"/>
     </row>
     <row r="383">
-      <c r="D383" s="72"/>
+      <c r="D383" s="79"/>
     </row>
     <row r="384">
-      <c r="D384" s="72"/>
+      <c r="D384" s="79"/>
     </row>
     <row r="385">
-      <c r="D385" s="72"/>
+      <c r="D385" s="79"/>
     </row>
     <row r="386">
-      <c r="D386" s="72"/>
+      <c r="D386" s="79"/>
     </row>
     <row r="387">
-      <c r="D387" s="72"/>
+      <c r="D387" s="79"/>
     </row>
     <row r="388">
-      <c r="D388" s="72"/>
+      <c r="D388" s="79"/>
     </row>
     <row r="389">
-      <c r="D389" s="72"/>
+      <c r="D389" s="79"/>
     </row>
     <row r="390">
-      <c r="D390" s="72"/>
+      <c r="D390" s="79"/>
     </row>
     <row r="391">
-      <c r="D391" s="72"/>
+      <c r="D391" s="79"/>
     </row>
     <row r="392">
-      <c r="D392" s="72"/>
+      <c r="D392" s="79"/>
     </row>
     <row r="393">
-      <c r="D393" s="72"/>
+      <c r="D393" s="79"/>
     </row>
     <row r="394">
-      <c r="D394" s="72"/>
+      <c r="D394" s="79"/>
     </row>
     <row r="395">
-      <c r="D395" s="72"/>
+      <c r="D395" s="79"/>
     </row>
     <row r="396">
-      <c r="D396" s="72"/>
+      <c r="D396" s="79"/>
     </row>
     <row r="397">
-      <c r="D397" s="72"/>
+      <c r="D397" s="79"/>
     </row>
     <row r="398">
-      <c r="D398" s="72"/>
+      <c r="D398" s="79"/>
     </row>
     <row r="399">
-      <c r="D399" s="72"/>
+      <c r="D399" s="79"/>
     </row>
     <row r="400">
-      <c r="D400" s="72"/>
+      <c r="D400" s="79"/>
     </row>
     <row r="401">
-      <c r="D401" s="72"/>
+      <c r="D401" s="79"/>
     </row>
     <row r="402">
-      <c r="D402" s="72"/>
+      <c r="D402" s="79"/>
     </row>
     <row r="403">
-      <c r="D403" s="72"/>
+      <c r="D403" s="79"/>
     </row>
     <row r="404">
-      <c r="D404" s="72"/>
+      <c r="D404" s="79"/>
     </row>
     <row r="405">
-      <c r="D405" s="72"/>
+      <c r="D405" s="79"/>
     </row>
     <row r="406">
-      <c r="D406" s="72"/>
+      <c r="D406" s="79"/>
     </row>
     <row r="407">
-      <c r="D407" s="72"/>
+      <c r="D407" s="79"/>
     </row>
     <row r="408">
-      <c r="D408" s="72"/>
+      <c r="D408" s="79"/>
     </row>
     <row r="409">
-      <c r="D409" s="72"/>
+      <c r="D409" s="79"/>
     </row>
     <row r="410">
-      <c r="D410" s="72"/>
+      <c r="D410" s="79"/>
     </row>
     <row r="411">
-      <c r="D411" s="72"/>
+      <c r="D411" s="79"/>
     </row>
     <row r="412">
-      <c r="D412" s="72"/>
+      <c r="D412" s="79"/>
     </row>
     <row r="413">
-      <c r="D413" s="72"/>
+      <c r="D413" s="79"/>
     </row>
     <row r="414">
-      <c r="D414" s="72"/>
+      <c r="D414" s="79"/>
     </row>
     <row r="415">
-      <c r="D415" s="72"/>
+      <c r="D415" s="79"/>
     </row>
     <row r="416">
-      <c r="D416" s="72"/>
+      <c r="D416" s="79"/>
     </row>
     <row r="417">
-      <c r="D417" s="72"/>
+      <c r="D417" s="79"/>
     </row>
     <row r="418">
-      <c r="D418" s="72"/>
+      <c r="D418" s="79"/>
     </row>
     <row r="419">
-      <c r="D419" s="72"/>
+      <c r="D419" s="79"/>
     </row>
     <row r="420">
-      <c r="D420" s="72"/>
+      <c r="D420" s="79"/>
     </row>
     <row r="421">
-      <c r="D421" s="72"/>
+      <c r="D421" s="79"/>
     </row>
     <row r="422">
-      <c r="D422" s="72"/>
+      <c r="D422" s="79"/>
     </row>
     <row r="423">
-      <c r="D423" s="72"/>
+      <c r="D423" s="79"/>
     </row>
     <row r="424">
-      <c r="D424" s="72"/>
+      <c r="D424" s="79"/>
     </row>
     <row r="425">
-      <c r="D425" s="72"/>
+      <c r="D425" s="79"/>
     </row>
     <row r="426">
-      <c r="D426" s="72"/>
+      <c r="D426" s="79"/>
     </row>
     <row r="427">
-      <c r="D427" s="72"/>
+      <c r="D427" s="79"/>
     </row>
     <row r="428">
-      <c r="D428" s="72"/>
+      <c r="D428" s="79"/>
     </row>
     <row r="429">
-      <c r="D429" s="72"/>
+      <c r="D429" s="79"/>
     </row>
     <row r="430">
-      <c r="D430" s="72"/>
+      <c r="D430" s="79"/>
     </row>
     <row r="431">
-      <c r="D431" s="72"/>
+      <c r="D431" s="79"/>
     </row>
     <row r="432">
-      <c r="D432" s="72"/>
+      <c r="D432" s="79"/>
     </row>
     <row r="433">
-      <c r="D433" s="72"/>
+      <c r="D433" s="79"/>
     </row>
     <row r="434">
-      <c r="D434" s="72"/>
+      <c r="D434" s="79"/>
     </row>
     <row r="435">
-      <c r="D435" s="72"/>
+      <c r="D435" s="79"/>
     </row>
     <row r="436">
-      <c r="D436" s="72"/>
+      <c r="D436" s="79"/>
     </row>
     <row r="437">
-      <c r="D437" s="72"/>
+      <c r="D437" s="79"/>
     </row>
     <row r="438">
-      <c r="D438" s="72"/>
+      <c r="D438" s="79"/>
     </row>
     <row r="439">
-      <c r="D439" s="72"/>
+      <c r="D439" s="79"/>
     </row>
     <row r="440">
-      <c r="D440" s="72"/>
+      <c r="D440" s="79"/>
     </row>
     <row r="441">
-      <c r="D441" s="72"/>
+      <c r="D441" s="79"/>
     </row>
     <row r="442">
-      <c r="D442" s="72"/>
+      <c r="D442" s="79"/>
     </row>
     <row r="443">
-      <c r="D443" s="72"/>
+      <c r="D443" s="79"/>
     </row>
     <row r="444">
-      <c r="D444" s="72"/>
+      <c r="D444" s="79"/>
     </row>
     <row r="445">
-      <c r="D445" s="72"/>
+      <c r="D445" s="79"/>
     </row>
     <row r="446">
-      <c r="D446" s="72"/>
+      <c r="D446" s="79"/>
     </row>
     <row r="447">
-      <c r="D447" s="72"/>
+      <c r="D447" s="79"/>
     </row>
     <row r="448">
-      <c r="D448" s="72"/>
+      <c r="D448" s="79"/>
     </row>
     <row r="449">
-      <c r="D449" s="72"/>
+      <c r="D449" s="79"/>
     </row>
     <row r="450">
-      <c r="D450" s="72"/>
+      <c r="D450" s="79"/>
     </row>
     <row r="451">
-      <c r="D451" s="72"/>
+      <c r="D451" s="79"/>
     </row>
     <row r="452">
-      <c r="D452" s="72"/>
+      <c r="D452" s="79"/>
     </row>
     <row r="453">
-      <c r="D453" s="72"/>
+      <c r="D453" s="79"/>
     </row>
     <row r="454">
-      <c r="D454" s="72"/>
+      <c r="D454" s="79"/>
     </row>
     <row r="455">
-      <c r="D455" s="72"/>
+      <c r="D455" s="79"/>
     </row>
     <row r="456">
-      <c r="D456" s="72"/>
+      <c r="D456" s="79"/>
     </row>
     <row r="457">
-      <c r="D457" s="72"/>
+      <c r="D457" s="79"/>
     </row>
     <row r="458">
-      <c r="D458" s="72"/>
+      <c r="D458" s="79"/>
     </row>
     <row r="459">
-      <c r="D459" s="72"/>
+      <c r="D459" s="79"/>
     </row>
     <row r="460">
-      <c r="D460" s="72"/>
+      <c r="D460" s="79"/>
     </row>
     <row r="461">
-      <c r="D461" s="72"/>
+      <c r="D461" s="79"/>
     </row>
     <row r="462">
-      <c r="D462" s="72"/>
+      <c r="D462" s="79"/>
     </row>
     <row r="463">
-      <c r="D463" s="72"/>
+      <c r="D463" s="79"/>
     </row>
     <row r="464">
-      <c r="D464" s="72"/>
+      <c r="D464" s="79"/>
     </row>
     <row r="465">
-      <c r="D465" s="72"/>
+      <c r="D465" s="79"/>
     </row>
     <row r="466">
-      <c r="D466" s="72"/>
+      <c r="D466" s="79"/>
     </row>
     <row r="467">
-      <c r="D467" s="72"/>
+      <c r="D467" s="79"/>
     </row>
     <row r="468">
-      <c r="D468" s="72"/>
+      <c r="D468" s="79"/>
     </row>
     <row r="469">
-      <c r="D469" s="72"/>
+      <c r="D469" s="79"/>
     </row>
     <row r="470">
-      <c r="D470" s="72"/>
+      <c r="D470" s="79"/>
     </row>
     <row r="471">
-      <c r="D471" s="72"/>
+      <c r="D471" s="79"/>
     </row>
     <row r="472">
-      <c r="D472" s="72"/>
+      <c r="D472" s="79"/>
     </row>
     <row r="473">
-      <c r="D473" s="72"/>
+      <c r="D473" s="79"/>
     </row>
     <row r="474">
-      <c r="D474" s="72"/>
+      <c r="D474" s="79"/>
     </row>
     <row r="475">
-      <c r="D475" s="72"/>
+      <c r="D475" s="79"/>
     </row>
     <row r="476">
-      <c r="D476" s="72"/>
+      <c r="D476" s="79"/>
     </row>
     <row r="477">
-      <c r="D477" s="72"/>
+      <c r="D477" s="79"/>
     </row>
     <row r="478">
-      <c r="D478" s="72"/>
+      <c r="D478" s="79"/>
     </row>
     <row r="479">
-      <c r="D479" s="72"/>
+      <c r="D479" s="79"/>
     </row>
     <row r="480">
-      <c r="D480" s="72"/>
+      <c r="D480" s="79"/>
     </row>
     <row r="481">
-      <c r="D481" s="72"/>
+      <c r="D481" s="79"/>
     </row>
     <row r="482">
-      <c r="D482" s="72"/>
+      <c r="D482" s="79"/>
     </row>
     <row r="483">
-      <c r="D483" s="72"/>
+      <c r="D483" s="79"/>
     </row>
     <row r="484">
-      <c r="D484" s="72"/>
+      <c r="D484" s="79"/>
     </row>
     <row r="485">
-      <c r="D485" s="72"/>
+      <c r="D485" s="79"/>
     </row>
     <row r="486">
-      <c r="D486" s="72"/>
+      <c r="D486" s="79"/>
     </row>
     <row r="487">
-      <c r="D487" s="72"/>
+      <c r="D487" s="79"/>
     </row>
     <row r="488">
-      <c r="D488" s="72"/>
+      <c r="D488" s="79"/>
     </row>
     <row r="489">
-      <c r="D489" s="72"/>
+      <c r="D489" s="79"/>
     </row>
     <row r="490">
-      <c r="D490" s="72"/>
+      <c r="D490" s="79"/>
     </row>
     <row r="491">
-      <c r="D491" s="72"/>
+      <c r="D491" s="79"/>
     </row>
     <row r="492">
-      <c r="D492" s="72"/>
+      <c r="D492" s="79"/>
     </row>
     <row r="493">
-      <c r="D493" s="72"/>
+      <c r="D493" s="79"/>
     </row>
     <row r="494">
-      <c r="D494" s="72"/>
+      <c r="D494" s="79"/>
     </row>
     <row r="495">
-      <c r="D495" s="72"/>
+      <c r="D495" s="79"/>
     </row>
     <row r="496">
-      <c r="D496" s="72"/>
+      <c r="D496" s="79"/>
     </row>
     <row r="497">
-      <c r="D497" s="72"/>
+      <c r="D497" s="79"/>
     </row>
     <row r="498">
-      <c r="D498" s="72"/>
+      <c r="D498" s="79"/>
     </row>
     <row r="499">
-      <c r="D499" s="72"/>
+      <c r="D499" s="79"/>
     </row>
     <row r="500">
-      <c r="D500" s="72"/>
+      <c r="D500" s="79"/>
     </row>
     <row r="501">
-      <c r="D501" s="72"/>
+      <c r="D501" s="79"/>
     </row>
     <row r="502">
-      <c r="D502" s="72"/>
+      <c r="D502" s="79"/>
     </row>
     <row r="503">
-      <c r="D503" s="72"/>
+      <c r="D503" s="79"/>
     </row>
     <row r="504">
-      <c r="D504" s="72"/>
+      <c r="D504" s="79"/>
     </row>
     <row r="505">
-      <c r="D505" s="72"/>
+      <c r="D505" s="79"/>
     </row>
     <row r="506">
-      <c r="D506" s="72"/>
+      <c r="D506" s="79"/>
     </row>
     <row r="507">
-      <c r="D507" s="72"/>
+      <c r="D507" s="79"/>
     </row>
     <row r="508">
-      <c r="D508" s="72"/>
+      <c r="D508" s="79"/>
     </row>
     <row r="509">
-      <c r="D509" s="72"/>
+      <c r="D509" s="79"/>
     </row>
     <row r="510">
-      <c r="D510" s="72"/>
+      <c r="D510" s="79"/>
     </row>
     <row r="511">
-      <c r="D511" s="72"/>
+      <c r="D511" s="79"/>
     </row>
     <row r="512">
-      <c r="D512" s="72"/>
+      <c r="D512" s="79"/>
     </row>
     <row r="513">
-      <c r="D513" s="72"/>
+      <c r="D513" s="79"/>
     </row>
     <row r="514">
-      <c r="D514" s="72"/>
+      <c r="D514" s="79"/>
     </row>
     <row r="515">
-      <c r="D515" s="72"/>
+      <c r="D515" s="79"/>
     </row>
     <row r="516">
-      <c r="D516" s="72"/>
+      <c r="D516" s="79"/>
     </row>
     <row r="517">
-      <c r="D517" s="72"/>
+      <c r="D517" s="79"/>
     </row>
     <row r="518">
-      <c r="D518" s="72"/>
+      <c r="D518" s="79"/>
     </row>
     <row r="519">
-      <c r="D519" s="72"/>
+      <c r="D519" s="79"/>
     </row>
     <row r="520">
-      <c r="D520" s="72"/>
+      <c r="D520" s="79"/>
     </row>
     <row r="521">
-      <c r="D521" s="72"/>
+      <c r="D521" s="79"/>
     </row>
     <row r="522">
-      <c r="D522" s="72"/>
+      <c r="D522" s="79"/>
     </row>
     <row r="523">
-      <c r="D523" s="72"/>
+      <c r="D523" s="79"/>
     </row>
     <row r="524">
-      <c r="D524" s="72"/>
+      <c r="D524" s="79"/>
     </row>
     <row r="525">
-      <c r="D525" s="72"/>
+      <c r="D525" s="79"/>
     </row>
     <row r="526">
-      <c r="D526" s="72"/>
+      <c r="D526" s="79"/>
     </row>
     <row r="527">
-      <c r="D527" s="72"/>
+      <c r="D527" s="79"/>
     </row>
     <row r="528">
-      <c r="D528" s="72"/>
+      <c r="D528" s="79"/>
     </row>
     <row r="529">
-      <c r="D529" s="72"/>
+      <c r="D529" s="79"/>
     </row>
     <row r="530">
-      <c r="D530" s="72"/>
+      <c r="D530" s="79"/>
     </row>
     <row r="531">
-      <c r="D531" s="72"/>
+      <c r="D531" s="79"/>
     </row>
     <row r="532">
-      <c r="D532" s="72"/>
+      <c r="D532" s="79"/>
     </row>
     <row r="533">
-      <c r="D533" s="72"/>
+      <c r="D533" s="79"/>
     </row>
     <row r="534">
-      <c r="D534" s="72"/>
+      <c r="D534" s="79"/>
     </row>
     <row r="535">
-      <c r="D535" s="72"/>
+      <c r="D535" s="79"/>
     </row>
     <row r="536">
-      <c r="D536" s="72"/>
+      <c r="D536" s="79"/>
     </row>
     <row r="537">
-      <c r="D537" s="72"/>
+      <c r="D537" s="79"/>
     </row>
     <row r="538">
-      <c r="D538" s="72"/>
+      <c r="D538" s="79"/>
     </row>
     <row r="539">
-      <c r="D539" s="72"/>
+      <c r="D539" s="79"/>
     </row>
     <row r="540">
-      <c r="D540" s="72"/>
+      <c r="D540" s="79"/>
     </row>
     <row r="541">
-      <c r="D541" s="72"/>
+      <c r="D541" s="79"/>
     </row>
     <row r="542">
-      <c r="D542" s="72"/>
+      <c r="D542" s="79"/>
     </row>
     <row r="543">
-      <c r="D543" s="72"/>
+      <c r="D543" s="79"/>
     </row>
     <row r="544">
-      <c r="D544" s="72"/>
+      <c r="D544" s="79"/>
     </row>
     <row r="545">
-      <c r="D545" s="72"/>
+      <c r="D545" s="79"/>
     </row>
     <row r="546">
-      <c r="D546" s="72"/>
+      <c r="D546" s="79"/>
     </row>
     <row r="547">
-      <c r="D547" s="72"/>
+      <c r="D547" s="79"/>
     </row>
     <row r="548">
-      <c r="D548" s="72"/>
+      <c r="D548" s="79"/>
     </row>
     <row r="549">
-      <c r="D549" s="72"/>
+      <c r="D549" s="79"/>
     </row>
     <row r="550">
-      <c r="D550" s="72"/>
+      <c r="D550" s="79"/>
     </row>
     <row r="551">
-      <c r="D551" s="72"/>
+      <c r="D551" s="79"/>
     </row>
     <row r="552">
-      <c r="D552" s="72"/>
+      <c r="D552" s="79"/>
     </row>
     <row r="553">
-      <c r="D553" s="72"/>
+      <c r="D553" s="79"/>
     </row>
     <row r="554">
-      <c r="D554" s="72"/>
+      <c r="D554" s="79"/>
     </row>
     <row r="555">
-      <c r="D555" s="72"/>
+      <c r="D555" s="79"/>
     </row>
     <row r="556">
-      <c r="D556" s="72"/>
+      <c r="D556" s="79"/>
     </row>
     <row r="557">
-      <c r="D557" s="72"/>
+      <c r="D557" s="79"/>
     </row>
     <row r="558">
-      <c r="D558" s="72"/>
+      <c r="D558" s="79"/>
     </row>
     <row r="559">
-      <c r="D559" s="72"/>
+      <c r="D559" s="79"/>
     </row>
     <row r="560">
-      <c r="D560" s="72"/>
+      <c r="D560" s="79"/>
     </row>
     <row r="561">
-      <c r="D561" s="72"/>
+      <c r="D561" s="79"/>
     </row>
     <row r="562">
-      <c r="D562" s="72"/>
+      <c r="D562" s="79"/>
     </row>
     <row r="563">
-      <c r="D563" s="72"/>
+      <c r="D563" s="79"/>
     </row>
     <row r="564">
-      <c r="D564" s="72"/>
+      <c r="D564" s="79"/>
     </row>
     <row r="565">
-      <c r="D565" s="72"/>
+      <c r="D565" s="79"/>
     </row>
     <row r="566">
-      <c r="D566" s="72"/>
+      <c r="D566" s="79"/>
     </row>
     <row r="567">
-      <c r="D567" s="72"/>
+      <c r="D567" s="79"/>
     </row>
     <row r="568">
-      <c r="D568" s="72"/>
+      <c r="D568" s="79"/>
     </row>
     <row r="569">
-      <c r="D569" s="72"/>
+      <c r="D569" s="79"/>
     </row>
     <row r="570">
-      <c r="D570" s="72"/>
+      <c r="D570" s="79"/>
     </row>
     <row r="571">
-      <c r="D571" s="72"/>
+      <c r="D571" s="79"/>
     </row>
     <row r="572">
-      <c r="D572" s="72"/>
+      <c r="D572" s="79"/>
     </row>
     <row r="573">
-      <c r="D573" s="72"/>
+      <c r="D573" s="79"/>
     </row>
     <row r="574">
-      <c r="D574" s="72"/>
+      <c r="D574" s="79"/>
     </row>
     <row r="575">
-      <c r="D575" s="72"/>
+      <c r="D575" s="79"/>
     </row>
     <row r="576">
-      <c r="D576" s="72"/>
+      <c r="D576" s="79"/>
     </row>
     <row r="577">
-      <c r="D577" s="72"/>
+      <c r="D577" s="79"/>
     </row>
     <row r="578">
-      <c r="D578" s="72"/>
+      <c r="D578" s="79"/>
     </row>
     <row r="579">
-      <c r="D579" s="72"/>
+      <c r="D579" s="79"/>
     </row>
     <row r="580">
-      <c r="D580" s="72"/>
+      <c r="D580" s="79"/>
     </row>
     <row r="581">
-      <c r="D581" s="72"/>
+      <c r="D581" s="79"/>
     </row>
     <row r="582">
-      <c r="D582" s="72"/>
+      <c r="D582" s="79"/>
     </row>
     <row r="583">
-      <c r="D583" s="72"/>
+      <c r="D583" s="79"/>
     </row>
     <row r="584">
-      <c r="D584" s="72"/>
+      <c r="D584" s="79"/>
     </row>
     <row r="585">
-      <c r="D585" s="72"/>
+      <c r="D585" s="79"/>
     </row>
     <row r="586">
-      <c r="D586" s="72"/>
+      <c r="D586" s="79"/>
     </row>
     <row r="587">
-      <c r="D587" s="72"/>
+      <c r="D587" s="79"/>
     </row>
     <row r="588">
-      <c r="D588" s="72"/>
+      <c r="D588" s="79"/>
     </row>
     <row r="589">
-      <c r="D589" s="72"/>
+      <c r="D589" s="79"/>
     </row>
     <row r="590">
-      <c r="D590" s="72"/>
+      <c r="D590" s="79"/>
     </row>
     <row r="591">
-      <c r="D591" s="72"/>
+      <c r="D591" s="79"/>
     </row>
     <row r="592">
-      <c r="D592" s="72"/>
+      <c r="D592" s="79"/>
     </row>
     <row r="593">
-      <c r="D593" s="72"/>
+      <c r="D593" s="79"/>
     </row>
     <row r="594">
-      <c r="D594" s="72"/>
+      <c r="D594" s="79"/>
     </row>
     <row r="595">
-      <c r="D595" s="72"/>
+      <c r="D595" s="79"/>
     </row>
     <row r="596">
-      <c r="D596" s="72"/>
+      <c r="D596" s="79"/>
     </row>
     <row r="597">
-      <c r="D597" s="72"/>
+      <c r="D597" s="79"/>
     </row>
     <row r="598">
-      <c r="D598" s="72"/>
+      <c r="D598" s="79"/>
     </row>
     <row r="599">
-      <c r="D599" s="72"/>
+      <c r="D599" s="79"/>
     </row>
     <row r="600">
-      <c r="D600" s="72"/>
+      <c r="D600" s="79"/>
     </row>
     <row r="601">
-      <c r="D601" s="72"/>
+      <c r="D601" s="79"/>
     </row>
     <row r="602">
-      <c r="D602" s="72"/>
+      <c r="D602" s="79"/>
     </row>
     <row r="603">
-      <c r="D603" s="72"/>
+      <c r="D603" s="79"/>
     </row>
     <row r="604">
-      <c r="D604" s="72"/>
+      <c r="D604" s="79"/>
     </row>
     <row r="605">
-      <c r="D605" s="72"/>
+      <c r="D605" s="79"/>
     </row>
     <row r="606">
-      <c r="D606" s="72"/>
+      <c r="D606" s="79"/>
     </row>
     <row r="607">
-      <c r="D607" s="72"/>
+      <c r="D607" s="79"/>
     </row>
     <row r="608">
-      <c r="D608" s="72"/>
+      <c r="D608" s="79"/>
     </row>
     <row r="609">
-      <c r="D609" s="72"/>
+      <c r="D609" s="79"/>
     </row>
     <row r="610">
-      <c r="D610" s="72"/>
+      <c r="D610" s="79"/>
     </row>
     <row r="611">
-      <c r="D611" s="72"/>
+      <c r="D611" s="79"/>
     </row>
     <row r="612">
-      <c r="D612" s="72"/>
+      <c r="D612" s="79"/>
     </row>
     <row r="613">
-      <c r="D613" s="72"/>
+      <c r="D613" s="79"/>
     </row>
     <row r="614">
-      <c r="D614" s="72"/>
+      <c r="D614" s="79"/>
     </row>
     <row r="615">
-      <c r="D615" s="72"/>
+      <c r="D615" s="79"/>
     </row>
     <row r="616">
-      <c r="D616" s="72"/>
+      <c r="D616" s="79"/>
     </row>
     <row r="617">
-      <c r="D617" s="72"/>
+      <c r="D617" s="79"/>
     </row>
     <row r="618">
-      <c r="D618" s="72"/>
+      <c r="D618" s="79"/>
     </row>
     <row r="619">
-      <c r="D619" s="72"/>
+      <c r="D619" s="79"/>
     </row>
     <row r="620">
-      <c r="D620" s="72"/>
+      <c r="D620" s="79"/>
     </row>
     <row r="621">
-      <c r="D621" s="72"/>
+      <c r="D621" s="79"/>
     </row>
     <row r="622">
-      <c r="D622" s="72"/>
+      <c r="D622" s="79"/>
     </row>
     <row r="623">
-      <c r="D623" s="72"/>
+      <c r="D623" s="79"/>
     </row>
     <row r="624">
-      <c r="D624" s="72"/>
+      <c r="D624" s="79"/>
     </row>
     <row r="625">
-      <c r="D625" s="72"/>
+      <c r="D625" s="79"/>
     </row>
     <row r="626">
-      <c r="D626" s="72"/>
+      <c r="D626" s="79"/>
     </row>
     <row r="627">
-      <c r="D627" s="72"/>
+      <c r="D627" s="79"/>
     </row>
     <row r="628">
-      <c r="D628" s="72"/>
+      <c r="D628" s="79"/>
     </row>
     <row r="629">
-      <c r="D629" s="72"/>
+      <c r="D629" s="79"/>
     </row>
     <row r="630">
-      <c r="D630" s="72"/>
+      <c r="D630" s="79"/>
     </row>
     <row r="631">
-      <c r="D631" s="72"/>
+      <c r="D631" s="79"/>
     </row>
     <row r="632">
-      <c r="D632" s="72"/>
+      <c r="D632" s="79"/>
     </row>
     <row r="633">
-      <c r="D633" s="72"/>
+      <c r="D633" s="79"/>
     </row>
     <row r="634">
-      <c r="D634" s="72"/>
+      <c r="D634" s="79"/>
     </row>
     <row r="635">
-      <c r="D635" s="72"/>
+      <c r="D635" s="79"/>
     </row>
     <row r="636">
-      <c r="D636" s="72"/>
+      <c r="D636" s="79"/>
     </row>
     <row r="637">
-      <c r="D637" s="72"/>
+      <c r="D637" s="79"/>
     </row>
     <row r="638">
-      <c r="D638" s="72"/>
+      <c r="D638" s="79"/>
     </row>
     <row r="639">
-      <c r="D639" s="72"/>
+      <c r="D639" s="79"/>
     </row>
     <row r="640">
-      <c r="D640" s="72"/>
+      <c r="D640" s="79"/>
     </row>
     <row r="641">
-      <c r="D641" s="72"/>
+      <c r="D641" s="79"/>
     </row>
     <row r="642">
-      <c r="D642" s="72"/>
+      <c r="D642" s="79"/>
     </row>
     <row r="643">
-      <c r="D643" s="72"/>
+      <c r="D643" s="79"/>
     </row>
     <row r="644">
-      <c r="D644" s="72"/>
+      <c r="D644" s="79"/>
     </row>
     <row r="645">
-      <c r="D645" s="72"/>
+      <c r="D645" s="79"/>
     </row>
     <row r="646">
-      <c r="D646" s="72"/>
+      <c r="D646" s="79"/>
     </row>
     <row r="647">
-      <c r="D647" s="72"/>
+      <c r="D647" s="79"/>
     </row>
     <row r="648">
-      <c r="D648" s="72"/>
+      <c r="D648" s="79"/>
     </row>
     <row r="649">
-      <c r="D649" s="72"/>
+      <c r="D649" s="79"/>
     </row>
     <row r="650">
-      <c r="D650" s="72"/>
+      <c r="D650" s="79"/>
     </row>
     <row r="651">
-      <c r="D651" s="72"/>
+      <c r="D651" s="79"/>
     </row>
     <row r="652">
-      <c r="D652" s="72"/>
+      <c r="D652" s="79"/>
     </row>
     <row r="653">
-      <c r="D653" s="72"/>
+      <c r="D653" s="79"/>
     </row>
     <row r="654">
-      <c r="D654" s="72"/>
+      <c r="D654" s="79"/>
     </row>
     <row r="655">
-      <c r="D655" s="72"/>
+      <c r="D655" s="79"/>
     </row>
     <row r="656">
-      <c r="D656" s="72"/>
+      <c r="D656" s="79"/>
     </row>
     <row r="657">
-      <c r="D657" s="72"/>
+      <c r="D657" s="79"/>
     </row>
     <row r="658">
-      <c r="D658" s="72"/>
+      <c r="D658" s="79"/>
     </row>
     <row r="659">
-      <c r="D659" s="72"/>
+      <c r="D659" s="79"/>
     </row>
     <row r="660">
-      <c r="D660" s="72"/>
+      <c r="D660" s="79"/>
     </row>
     <row r="661">
-      <c r="D661" s="72"/>
+      <c r="D661" s="79"/>
     </row>
     <row r="662">
-      <c r="D662" s="72"/>
+      <c r="D662" s="79"/>
     </row>
     <row r="663">
-      <c r="D663" s="72"/>
+      <c r="D663" s="79"/>
     </row>
     <row r="664">
-      <c r="D664" s="72"/>
+      <c r="D664" s="79"/>
     </row>
     <row r="665">
-      <c r="D665" s="72"/>
+      <c r="D665" s="79"/>
     </row>
     <row r="666">
-      <c r="D666" s="72"/>
+      <c r="D666" s="79"/>
     </row>
     <row r="667">
-      <c r="D667" s="72"/>
+      <c r="D667" s="79"/>
     </row>
     <row r="668">
-      <c r="D668" s="72"/>
+      <c r="D668" s="79"/>
     </row>
     <row r="669">
-      <c r="D669" s="72"/>
+      <c r="D669" s="79"/>
     </row>
     <row r="670">
-      <c r="D670" s="72"/>
+      <c r="D670" s="79"/>
     </row>
     <row r="671">
-      <c r="D671" s="72"/>
+      <c r="D671" s="79"/>
     </row>
     <row r="672">
-      <c r="D672" s="72"/>
+      <c r="D672" s="79"/>
     </row>
     <row r="673">
-      <c r="D673" s="72"/>
+      <c r="D673" s="79"/>
     </row>
     <row r="674">
-      <c r="D674" s="72"/>
+      <c r="D674" s="79"/>
     </row>
     <row r="675">
-      <c r="D675" s="72"/>
+      <c r="D675" s="79"/>
     </row>
     <row r="676">
-      <c r="D676" s="72"/>
+      <c r="D676" s="79"/>
     </row>
     <row r="677">
-      <c r="D677" s="72"/>
+      <c r="D677" s="79"/>
     </row>
     <row r="678">
-      <c r="D678" s="72"/>
+      <c r="D678" s="79"/>
     </row>
     <row r="679">
-      <c r="D679" s="72"/>
+      <c r="D679" s="79"/>
     </row>
     <row r="680">
-      <c r="D680" s="72"/>
+      <c r="D680" s="79"/>
     </row>
     <row r="681">
-      <c r="D681" s="72"/>
+      <c r="D681" s="79"/>
     </row>
     <row r="682">
-      <c r="D682" s="72"/>
+      <c r="D682" s="79"/>
     </row>
     <row r="683">
-      <c r="D683" s="72"/>
+      <c r="D683" s="79"/>
     </row>
     <row r="684">
-      <c r="D684" s="72"/>
+      <c r="D684" s="79"/>
     </row>
     <row r="685">
-      <c r="D685" s="72"/>
+      <c r="D685" s="79"/>
     </row>
     <row r="686">
-      <c r="D686" s="72"/>
+      <c r="D686" s="79"/>
     </row>
     <row r="687">
-      <c r="D687" s="72"/>
+      <c r="D687" s="79"/>
     </row>
     <row r="688">
-      <c r="D688" s="72"/>
+      <c r="D688" s="79"/>
     </row>
     <row r="689">
-      <c r="D689" s="72"/>
+      <c r="D689" s="79"/>
     </row>
     <row r="690">
-      <c r="D690" s="72"/>
+      <c r="D690" s="79"/>
     </row>
     <row r="691">
-      <c r="D691" s="72"/>
+      <c r="D691" s="79"/>
     </row>
     <row r="692">
-      <c r="D692" s="72"/>
+      <c r="D692" s="79"/>
     </row>
     <row r="693">
-      <c r="D693" s="72"/>
+      <c r="D693" s="79"/>
     </row>
     <row r="694">
-      <c r="D694" s="72"/>
+      <c r="D694" s="79"/>
     </row>
     <row r="695">
-      <c r="D695" s="72"/>
+      <c r="D695" s="79"/>
     </row>
     <row r="696">
-      <c r="D696" s="72"/>
+      <c r="D696" s="79"/>
     </row>
     <row r="697">
-      <c r="D697" s="72"/>
+      <c r="D697" s="79"/>
     </row>
     <row r="698">
-      <c r="D698" s="72"/>
+      <c r="D698" s="79"/>
     </row>
     <row r="699">
-      <c r="D699" s="72"/>
+      <c r="D699" s="79"/>
     </row>
     <row r="700">
-      <c r="D700" s="72"/>
+      <c r="D700" s="79"/>
     </row>
     <row r="701">
-      <c r="D701" s="72"/>
+      <c r="D701" s="79"/>
     </row>
     <row r="702">
-      <c r="D702" s="72"/>
+      <c r="D702" s="79"/>
     </row>
     <row r="703">
-      <c r="D703" s="72"/>
+      <c r="D703" s="79"/>
     </row>
     <row r="704">
-      <c r="D704" s="72"/>
+      <c r="D704" s="79"/>
     </row>
     <row r="705">
-      <c r="D705" s="72"/>
+      <c r="D705" s="79"/>
     </row>
     <row r="706">
-      <c r="D706" s="72"/>
+      <c r="D706" s="79"/>
     </row>
     <row r="707">
-      <c r="D707" s="72"/>
+      <c r="D707" s="79"/>
     </row>
     <row r="708">
-      <c r="D708" s="72"/>
+      <c r="D708" s="79"/>
     </row>
     <row r="709">
-      <c r="D709" s="72"/>
+      <c r="D709" s="79"/>
     </row>
     <row r="710">
-      <c r="D710" s="72"/>
+      <c r="D710" s="79"/>
     </row>
     <row r="711">
-      <c r="D711" s="72"/>
+      <c r="D711" s="79"/>
     </row>
     <row r="712">
-      <c r="D712" s="72"/>
+      <c r="D712" s="79"/>
     </row>
     <row r="713">
-      <c r="D713" s="72"/>
+      <c r="D713" s="79"/>
     </row>
     <row r="714">
-      <c r="D714" s="72"/>
+      <c r="D714" s="79"/>
     </row>
     <row r="715">
-      <c r="D715" s="72"/>
+      <c r="D715" s="79"/>
     </row>
     <row r="716">
-      <c r="D716" s="72"/>
+      <c r="D716" s="79"/>
     </row>
     <row r="717">
-      <c r="D717" s="72"/>
+      <c r="D717" s="79"/>
     </row>
     <row r="718">
-      <c r="D718" s="72"/>
+      <c r="D718" s="79"/>
     </row>
     <row r="719">
-      <c r="D719" s="72"/>
+      <c r="D719" s="79"/>
     </row>
     <row r="720">
-      <c r="D720" s="72"/>
+      <c r="D720" s="79"/>
     </row>
     <row r="721">
-      <c r="D721" s="72"/>
+      <c r="D721" s="79"/>
     </row>
     <row r="722">
-      <c r="D722" s="72"/>
+      <c r="D722" s="79"/>
     </row>
     <row r="723">
-      <c r="D723" s="72"/>
+      <c r="D723" s="79"/>
     </row>
     <row r="724">
-      <c r="D724" s="72"/>
+      <c r="D724" s="79"/>
     </row>
     <row r="725">
-      <c r="D725" s="72"/>
+      <c r="D725" s="79"/>
     </row>
     <row r="726">
-      <c r="D726" s="72"/>
+      <c r="D726" s="79"/>
     </row>
     <row r="727">
-      <c r="D727" s="72"/>
+      <c r="D727" s="79"/>
     </row>
     <row r="728">
-      <c r="D728" s="72"/>
+      <c r="D728" s="79"/>
     </row>
     <row r="729">
-      <c r="D729" s="72"/>
+      <c r="D729" s="79"/>
     </row>
     <row r="730">
-      <c r="D730" s="72"/>
+      <c r="D730" s="79"/>
     </row>
     <row r="731">
-      <c r="D731" s="72"/>
+      <c r="D731" s="79"/>
     </row>
     <row r="732">
-      <c r="D732" s="72"/>
+      <c r="D732" s="79"/>
     </row>
     <row r="733">
-      <c r="D733" s="72"/>
+      <c r="D733" s="79"/>
     </row>
     <row r="734">
-      <c r="D734" s="72"/>
+      <c r="D734" s="79"/>
     </row>
     <row r="735">
-      <c r="D735" s="72"/>
+      <c r="D735" s="79"/>
     </row>
     <row r="736">
-      <c r="D736" s="72"/>
+      <c r="D736" s="79"/>
     </row>
     <row r="737">
-      <c r="D737" s="72"/>
+      <c r="D737" s="79"/>
     </row>
     <row r="738">
-      <c r="D738" s="72"/>
+      <c r="D738" s="79"/>
     </row>
     <row r="739">
-      <c r="D739" s="72"/>
+      <c r="D739" s="79"/>
     </row>
     <row r="740">
-      <c r="D740" s="72"/>
+      <c r="D740" s="79"/>
     </row>
     <row r="741">
-      <c r="D741" s="72"/>
+      <c r="D741" s="79"/>
     </row>
     <row r="742">
-      <c r="D742" s="72"/>
+      <c r="D742" s="79"/>
     </row>
     <row r="743">
-      <c r="D743" s="72"/>
+      <c r="D743" s="79"/>
     </row>
     <row r="744">
-      <c r="D744" s="72"/>
+      <c r="D744" s="79"/>
     </row>
     <row r="745">
-      <c r="D745" s="72"/>
+      <c r="D745" s="79"/>
     </row>
     <row r="746">
-      <c r="D746" s="72"/>
+      <c r="D746" s="79"/>
     </row>
     <row r="747">
-      <c r="D747" s="72"/>
+      <c r="D747" s="79"/>
     </row>
     <row r="748">
-      <c r="D748" s="72"/>
+      <c r="D748" s="79"/>
     </row>
     <row r="749">
-      <c r="D749" s="72"/>
+      <c r="D749" s="79"/>
     </row>
     <row r="750">
-      <c r="D750" s="72"/>
+      <c r="D750" s="79"/>
     </row>
     <row r="751">
-      <c r="D751" s="72"/>
+      <c r="D751" s="79"/>
     </row>
     <row r="752">
-      <c r="D752" s="72"/>
+      <c r="D752" s="79"/>
     </row>
     <row r="753">
-      <c r="D753" s="72"/>
+      <c r="D753" s="79"/>
     </row>
     <row r="754">
-      <c r="D754" s="72"/>
+      <c r="D754" s="79"/>
     </row>
     <row r="755">
-      <c r="D755" s="72"/>
+      <c r="D755" s="79"/>
     </row>
     <row r="756">
-      <c r="D756" s="72"/>
+      <c r="D756" s="79"/>
     </row>
     <row r="757">
-      <c r="D757" s="72"/>
+      <c r="D757" s="79"/>
     </row>
     <row r="758">
-      <c r="D758" s="72"/>
+      <c r="D758" s="79"/>
     </row>
     <row r="759">
-      <c r="D759" s="72"/>
+      <c r="D759" s="79"/>
     </row>
     <row r="760">
-      <c r="D760" s="72"/>
+      <c r="D760" s="79"/>
     </row>
     <row r="761">
-      <c r="D761" s="72"/>
+      <c r="D761" s="79"/>
     </row>
     <row r="762">
-      <c r="D762" s="72"/>
+      <c r="D762" s="79"/>
     </row>
     <row r="763">
-      <c r="D763" s="72"/>
+      <c r="D763" s="79"/>
     </row>
     <row r="764">
-      <c r="D764" s="72"/>
+      <c r="D764" s="79"/>
     </row>
     <row r="765">
-      <c r="D765" s="72"/>
+      <c r="D765" s="79"/>
     </row>
     <row r="766">
-      <c r="D766" s="72"/>
+      <c r="D766" s="79"/>
     </row>
     <row r="767">
-      <c r="D767" s="72"/>
+      <c r="D767" s="79"/>
     </row>
     <row r="768">
-      <c r="D768" s="72"/>
+      <c r="D768" s="79"/>
     </row>
     <row r="769">
-      <c r="D769" s="72"/>
+      <c r="D769" s="79"/>
     </row>
     <row r="770">
-      <c r="D770" s="72"/>
+      <c r="D770" s="79"/>
     </row>
     <row r="771">
-      <c r="D771" s="72"/>
+      <c r="D771" s="79"/>
     </row>
     <row r="772">
-      <c r="D772" s="72"/>
+      <c r="D772" s="79"/>
     </row>
     <row r="773">
-      <c r="D773" s="72"/>
+      <c r="D773" s="79"/>
     </row>
     <row r="774">
-      <c r="D774" s="72"/>
+      <c r="D774" s="79"/>
     </row>
     <row r="775">
-      <c r="D775" s="72"/>
+      <c r="D775" s="79"/>
     </row>
     <row r="776">
-      <c r="D776" s="72"/>
+      <c r="D776" s="79"/>
     </row>
     <row r="777">
-      <c r="D777" s="72"/>
+      <c r="D777" s="79"/>
     </row>
     <row r="778">
-      <c r="D778" s="72"/>
+      <c r="D778" s="79"/>
     </row>
     <row r="779">
-      <c r="D779" s="72"/>
+      <c r="D779" s="79"/>
     </row>
     <row r="780">
-      <c r="D780" s="72"/>
+      <c r="D780" s="79"/>
     </row>
     <row r="781">
-      <c r="D781" s="72"/>
+      <c r="D781" s="79"/>
     </row>
     <row r="782">
-      <c r="D782" s="72"/>
+      <c r="D782" s="79"/>
     </row>
     <row r="783">
-      <c r="D783" s="72"/>
+      <c r="D783" s="79"/>
     </row>
     <row r="784">
-      <c r="D784" s="72"/>
+      <c r="D784" s="79"/>
     </row>
     <row r="785">
-      <c r="D785" s="72"/>
+      <c r="D785" s="79"/>
     </row>
     <row r="786">
-      <c r="D786" s="72"/>
+      <c r="D786" s="79"/>
     </row>
     <row r="787">
-      <c r="D787" s="72"/>
+      <c r="D787" s="79"/>
     </row>
     <row r="788">
-      <c r="D788" s="72"/>
+      <c r="D788" s="79"/>
     </row>
     <row r="789">
-      <c r="D789" s="72"/>
+      <c r="D789" s="79"/>
     </row>
     <row r="790">
-      <c r="D790" s="72"/>
+      <c r="D790" s="79"/>
     </row>
     <row r="791">
-      <c r="D791" s="72"/>
+      <c r="D791" s="79"/>
     </row>
     <row r="792">
-      <c r="D792" s="72"/>
+      <c r="D792" s="79"/>
     </row>
     <row r="793">
-      <c r="D793" s="72"/>
+      <c r="D793" s="79"/>
     </row>
     <row r="794">
-      <c r="D794" s="72"/>
+      <c r="D794" s="79"/>
     </row>
     <row r="795">
-      <c r="D795" s="72"/>
+      <c r="D795" s="79"/>
     </row>
     <row r="796">
-      <c r="D796" s="72"/>
+      <c r="D796" s="79"/>
     </row>
     <row r="797">
-      <c r="D797" s="72"/>
+      <c r="D797" s="79"/>
     </row>
     <row r="798">
-      <c r="D798" s="72"/>
+      <c r="D798" s="79"/>
     </row>
     <row r="799">
-      <c r="D799" s="72"/>
+      <c r="D799" s="79"/>
     </row>
     <row r="800">
-      <c r="D800" s="72"/>
+      <c r="D800" s="79"/>
     </row>
     <row r="801">
-      <c r="D801" s="72"/>
+      <c r="D801" s="79"/>
     </row>
     <row r="802">
-      <c r="D802" s="72"/>
+      <c r="D802" s="79"/>
     </row>
     <row r="803">
-      <c r="D803" s="72"/>
+      <c r="D803" s="79"/>
     </row>
     <row r="804">
-      <c r="D804" s="72"/>
+      <c r="D804" s="79"/>
     </row>
     <row r="805">
-      <c r="D805" s="72"/>
+      <c r="D805" s="79"/>
     </row>
     <row r="806">
-      <c r="D806" s="72"/>
+      <c r="D806" s="79"/>
     </row>
     <row r="807">
-      <c r="D807" s="72"/>
+      <c r="D807" s="79"/>
     </row>
     <row r="808">
-      <c r="D808" s="72"/>
+      <c r="D808" s="79"/>
     </row>
     <row r="809">
-      <c r="D809" s="72"/>
+      <c r="D809" s="79"/>
     </row>
     <row r="810">
-      <c r="D810" s="72"/>
+      <c r="D810" s="79"/>
     </row>
     <row r="811">
-      <c r="D811" s="72"/>
+      <c r="D811" s="79"/>
     </row>
     <row r="812">
-      <c r="D812" s="72"/>
+      <c r="D812" s="79"/>
     </row>
     <row r="813">
-      <c r="D813" s="72"/>
+      <c r="D813" s="79"/>
     </row>
     <row r="814">
-      <c r="D814" s="72"/>
+      <c r="D814" s="79"/>
     </row>
     <row r="815">
-      <c r="D815" s="72"/>
+      <c r="D815" s="79"/>
     </row>
     <row r="816">
-      <c r="D816" s="72"/>
+      <c r="D816" s="79"/>
     </row>
     <row r="817">
-      <c r="D817" s="72"/>
+      <c r="D817" s="79"/>
     </row>
     <row r="818">
-      <c r="D818" s="72"/>
+      <c r="D818" s="79"/>
     </row>
     <row r="819">
-      <c r="D819" s="72"/>
+      <c r="D819" s="79"/>
     </row>
     <row r="820">
-      <c r="D820" s="72"/>
+      <c r="D820" s="79"/>
     </row>
     <row r="821">
-      <c r="D821" s="72"/>
+      <c r="D821" s="79"/>
     </row>
     <row r="822">
-      <c r="D822" s="72"/>
+      <c r="D822" s="79"/>
     </row>
     <row r="823">
-      <c r="D823" s="72"/>
+      <c r="D823" s="79"/>
     </row>
     <row r="824">
-      <c r="D824" s="72"/>
+      <c r="D824" s="79"/>
     </row>
     <row r="825">
-      <c r="D825" s="72"/>
+      <c r="D825" s="79"/>
     </row>
     <row r="826">
-      <c r="D826" s="72"/>
+      <c r="D826" s="79"/>
     </row>
     <row r="827">
-      <c r="D827" s="72"/>
+      <c r="D827" s="79"/>
     </row>
     <row r="828">
-      <c r="D828" s="72"/>
+      <c r="D828" s="79"/>
     </row>
     <row r="829">
-      <c r="D829" s="72"/>
+      <c r="D829" s="79"/>
     </row>
     <row r="830">
-      <c r="D830" s="72"/>
+      <c r="D830" s="79"/>
     </row>
     <row r="831">
-      <c r="D831" s="72"/>
+      <c r="D831" s="79"/>
     </row>
     <row r="832">
-      <c r="D832" s="72"/>
+      <c r="D832" s="79"/>
     </row>
     <row r="833">
-      <c r="D833" s="72"/>
+      <c r="D833" s="79"/>
     </row>
     <row r="834">
-      <c r="D834" s="72"/>
+      <c r="D834" s="79"/>
     </row>
     <row r="835">
-      <c r="D835" s="72"/>
+      <c r="D835" s="79"/>
     </row>
     <row r="836">
-      <c r="D836" s="72"/>
+      <c r="D836" s="79"/>
     </row>
     <row r="837">
-      <c r="D837" s="72"/>
+      <c r="D837" s="79"/>
     </row>
     <row r="838">
-      <c r="D838" s="72"/>
+      <c r="D838" s="79"/>
     </row>
     <row r="839">
-      <c r="D839" s="72"/>
+      <c r="D839" s="79"/>
     </row>
     <row r="840">
-      <c r="D840" s="72"/>
+      <c r="D840" s="79"/>
     </row>
     <row r="841">
-      <c r="D841" s="72"/>
+      <c r="D841" s="79"/>
     </row>
     <row r="842">
-      <c r="D842" s="72"/>
+      <c r="D842" s="79"/>
     </row>
     <row r="843">
-      <c r="D843" s="72"/>
+      <c r="D843" s="79"/>
     </row>
     <row r="844">
-      <c r="D844" s="72"/>
+      <c r="D844" s="79"/>
     </row>
     <row r="845">
-      <c r="D845" s="72"/>
+      <c r="D845" s="79"/>
     </row>
     <row r="846">
-      <c r="D846" s="72"/>
+      <c r="D846" s="79"/>
     </row>
     <row r="847">
-      <c r="D847" s="72"/>
+      <c r="D847" s="79"/>
     </row>
     <row r="848">
-      <c r="D848" s="72"/>
+      <c r="D848" s="79"/>
     </row>
     <row r="849">
-      <c r="D849" s="72"/>
+      <c r="D849" s="79"/>
     </row>
     <row r="850">
-      <c r="D850" s="72"/>
+      <c r="D850" s="79"/>
     </row>
     <row r="851">
-      <c r="D851" s="72"/>
+      <c r="D851" s="79"/>
     </row>
     <row r="852">
-      <c r="D852" s="72"/>
+      <c r="D852" s="79"/>
     </row>
     <row r="853">
-      <c r="D853" s="72"/>
+      <c r="D853" s="79"/>
     </row>
     <row r="854">
-      <c r="D854" s="72"/>
+      <c r="D854" s="79"/>
     </row>
     <row r="855">
-      <c r="D855" s="72"/>
+      <c r="D855" s="79"/>
     </row>
     <row r="856">
-      <c r="D856" s="72"/>
+      <c r="D856" s="79"/>
     </row>
     <row r="857">
-      <c r="D857" s="72"/>
+      <c r="D857" s="79"/>
     </row>
     <row r="858">
-      <c r="D858" s="72"/>
+      <c r="D858" s="79"/>
     </row>
     <row r="859">
-      <c r="D859" s="72"/>
+      <c r="D859" s="79"/>
     </row>
     <row r="860">
-      <c r="D860" s="72"/>
+      <c r="D860" s="79"/>
     </row>
     <row r="861">
-      <c r="D861" s="72"/>
+      <c r="D861" s="79"/>
     </row>
     <row r="862">
-      <c r="D862" s="72"/>
+      <c r="D862" s="79"/>
     </row>
     <row r="863">
-      <c r="D863" s="72"/>
+      <c r="D863" s="79"/>
     </row>
     <row r="864">
-      <c r="D864" s="72"/>
+      <c r="D864" s="79"/>
     </row>
     <row r="865">
-      <c r="D865" s="72"/>
+      <c r="D865" s="79"/>
     </row>
     <row r="866">
-      <c r="D866" s="72"/>
+      <c r="D866" s="79"/>
     </row>
     <row r="867">
-      <c r="D867" s="72"/>
+      <c r="D867" s="79"/>
     </row>
     <row r="868">
-      <c r="D868" s="72"/>
+      <c r="D868" s="79"/>
     </row>
     <row r="869">
-      <c r="D869" s="72"/>
+      <c r="D869" s="79"/>
     </row>
     <row r="870">
-      <c r="D870" s="72"/>
+      <c r="D870" s="79"/>
     </row>
     <row r="871">
-      <c r="D871" s="72"/>
+      <c r="D871" s="79"/>
     </row>
     <row r="872">
-      <c r="D872" s="72"/>
+      <c r="D872" s="79"/>
     </row>
     <row r="873">
-      <c r="D873" s="72"/>
+      <c r="D873" s="79"/>
     </row>
     <row r="874">
-      <c r="D874" s="72"/>
+      <c r="D874" s="79"/>
     </row>
     <row r="875">
-      <c r="D875" s="72"/>
+      <c r="D875" s="79"/>
     </row>
     <row r="876">
-      <c r="D876" s="72"/>
+      <c r="D876" s="79"/>
     </row>
     <row r="877">
-      <c r="D877" s="72"/>
+      <c r="D877" s="79"/>
     </row>
     <row r="878">
-      <c r="D878" s="72"/>
+      <c r="D878" s="79"/>
     </row>
     <row r="879">
-      <c r="D879" s="72"/>
+      <c r="D879" s="79"/>
     </row>
     <row r="880">
-      <c r="D880" s="72"/>
+      <c r="D880" s="79"/>
     </row>
     <row r="881">
-      <c r="D881" s="72"/>
+      <c r="D881" s="79"/>
     </row>
     <row r="882">
-      <c r="D882" s="72"/>
+      <c r="D882" s="79"/>
     </row>
     <row r="883">
-      <c r="D883" s="72"/>
+      <c r="D883" s="79"/>
     </row>
     <row r="884">
-      <c r="D884" s="72"/>
+      <c r="D884" s="79"/>
     </row>
     <row r="885">
-      <c r="D885" s="72"/>
+      <c r="D885" s="79"/>
     </row>
     <row r="886">
-      <c r="D886" s="72"/>
+      <c r="D886" s="79"/>
     </row>
     <row r="887">
-      <c r="D887" s="72"/>
+      <c r="D887" s="79"/>
     </row>
     <row r="888">
-      <c r="D888" s="72"/>
+      <c r="D888" s="79"/>
     </row>
     <row r="889">
-      <c r="D889" s="72"/>
+      <c r="D889" s="79"/>
     </row>
     <row r="890">
-      <c r="D890" s="72"/>
+      <c r="D890" s="79"/>
     </row>
     <row r="891">
-      <c r="D891" s="72"/>
+      <c r="D891" s="79"/>
     </row>
     <row r="892">
-      <c r="D892" s="72"/>
+      <c r="D892" s="79"/>
     </row>
     <row r="893">
-      <c r="D893" s="72"/>
+      <c r="D893" s="79"/>
     </row>
     <row r="894">
-      <c r="D894" s="72"/>
+      <c r="D894" s="79"/>
     </row>
     <row r="895">
-      <c r="D895" s="72"/>
+      <c r="D895" s="79"/>
     </row>
     <row r="896">
-      <c r="D896" s="72"/>
+      <c r="D896" s="79"/>
     </row>
     <row r="897">
-      <c r="D897" s="72"/>
+      <c r="D897" s="79"/>
     </row>
     <row r="898">
-      <c r="D898" s="72"/>
+      <c r="D898" s="79"/>
     </row>
     <row r="899">
-      <c r="D899" s="72"/>
+      <c r="D899" s="79"/>
     </row>
     <row r="900">
-      <c r="D900" s="72"/>
+      <c r="D900" s="79"/>
     </row>
     <row r="901">
-      <c r="D901" s="72"/>
+      <c r="D901" s="79"/>
     </row>
     <row r="902">
-      <c r="D902" s="72"/>
+      <c r="D902" s="79"/>
     </row>
     <row r="903">
-      <c r="D903" s="72"/>
+      <c r="D903" s="79"/>
     </row>
     <row r="904">
-      <c r="D904" s="72"/>
+      <c r="D904" s="79"/>
     </row>
     <row r="905">
-      <c r="D905" s="72"/>
+      <c r="D905" s="79"/>
     </row>
     <row r="906">
-      <c r="D906" s="72"/>
+      <c r="D906" s="79"/>
     </row>
     <row r="907">
-      <c r="D907" s="72"/>
+      <c r="D907" s="79"/>
     </row>
     <row r="908">
-      <c r="D908" s="72"/>
+      <c r="D908" s="79"/>
     </row>
     <row r="909">
-      <c r="D909" s="72"/>
+      <c r="D909" s="79"/>
     </row>
     <row r="910">
-      <c r="D910" s="72"/>
+      <c r="D910" s="79"/>
     </row>
     <row r="911">
-      <c r="D911" s="72"/>
+      <c r="D911" s="79"/>
     </row>
     <row r="912">
-      <c r="D912" s="72"/>
+      <c r="D912" s="79"/>
     </row>
     <row r="913">
-      <c r="D913" s="72"/>
+      <c r="D913" s="79"/>
     </row>
     <row r="914">
-      <c r="D914" s="72"/>
+      <c r="D914" s="79"/>
     </row>
     <row r="915">
-      <c r="D915" s="72"/>
+      <c r="D915" s="79"/>
     </row>
     <row r="916">
-      <c r="D916" s="72"/>
+      <c r="D916" s="79"/>
     </row>
     <row r="917">
-      <c r="D917" s="72"/>
+      <c r="D917" s="79"/>
     </row>
     <row r="918">
-      <c r="D918" s="72"/>
+      <c r="D918" s="79"/>
     </row>
     <row r="919">
-      <c r="D919" s="72"/>
+      <c r="D919" s="79"/>
     </row>
     <row r="920">
-      <c r="D920" s="72"/>
+      <c r="D920" s="79"/>
     </row>
     <row r="921">
-      <c r="D921" s="72"/>
+      <c r="D921" s="79"/>
     </row>
     <row r="922">
-      <c r="D922" s="72"/>
+      <c r="D922" s="79"/>
     </row>
     <row r="923">
-      <c r="D923" s="72"/>
+      <c r="D923" s="79"/>
     </row>
     <row r="924">
-      <c r="D924" s="72"/>
+      <c r="D924" s="79"/>
     </row>
     <row r="925">
-      <c r="D925" s="72"/>
+      <c r="D925" s="79"/>
     </row>
     <row r="926">
-      <c r="D926" s="72"/>
+      <c r="D926" s="79"/>
     </row>
     <row r="927">
-      <c r="D927" s="72"/>
+      <c r="D927" s="79"/>
     </row>
     <row r="928">
-      <c r="D928" s="72"/>
+      <c r="D928" s="79"/>
     </row>
     <row r="929">
-      <c r="D929" s="72"/>
+      <c r="D929" s="79"/>
     </row>
     <row r="930">
-      <c r="D930" s="72"/>
+      <c r="D930" s="79"/>
     </row>
     <row r="931">
-      <c r="D931" s="72"/>
+      <c r="D931" s="79"/>
     </row>
     <row r="932">
-      <c r="D932" s="72"/>
+      <c r="D932" s="79"/>
     </row>
     <row r="933">
-      <c r="D933" s="72"/>
+      <c r="D933" s="79"/>
     </row>
     <row r="934">
-      <c r="D934" s="72"/>
+      <c r="D934" s="79"/>
     </row>
     <row r="935">
-      <c r="D935" s="72"/>
+      <c r="D935" s="79"/>
     </row>
     <row r="936">
-      <c r="D936" s="72"/>
+      <c r="D936" s="79"/>
     </row>
     <row r="937">
-      <c r="D937" s="72"/>
+      <c r="D937" s="79"/>
     </row>
     <row r="938">
-      <c r="D938" s="72"/>
+      <c r="D938" s="79"/>
     </row>
     <row r="939">
-      <c r="D939" s="72"/>
+      <c r="D939" s="79"/>
     </row>
     <row r="940">
-      <c r="D940" s="72"/>
+      <c r="D940" s="79"/>
     </row>
     <row r="941">
-      <c r="D941" s="72"/>
+      <c r="D941" s="79"/>
     </row>
     <row r="942">
-      <c r="D942" s="72"/>
+      <c r="D942" s="79"/>
     </row>
     <row r="943">
-      <c r="D943" s="72"/>
+      <c r="D943" s="79"/>
     </row>
     <row r="944">
-      <c r="D944" s="72"/>
+      <c r="D944" s="79"/>
     </row>
     <row r="945">
-      <c r="D945" s="72"/>
+      <c r="D945" s="79"/>
     </row>
     <row r="946">
-      <c r="D946" s="72"/>
+      <c r="D946" s="79"/>
     </row>
     <row r="947">
-      <c r="D947" s="72"/>
+      <c r="D947" s="79"/>
     </row>
     <row r="948">
-      <c r="D948" s="72"/>
+      <c r="D948" s="79"/>
     </row>
     <row r="949">
-      <c r="D949" s="72"/>
+      <c r="D949" s="79"/>
     </row>
     <row r="950">
-      <c r="D950" s="72"/>
+      <c r="D950" s="79"/>
     </row>
     <row r="951">
-      <c r="D951" s="72"/>
+      <c r="D951" s="79"/>
     </row>
     <row r="952">
-      <c r="D952" s="72"/>
+      <c r="D952" s="79"/>
     </row>
     <row r="953">
-      <c r="D953" s="72"/>
+      <c r="D953" s="79"/>
     </row>
     <row r="954">
-      <c r="D954" s="72"/>
+      <c r="D954" s="79"/>
     </row>
     <row r="955">
-      <c r="D955" s="72"/>
+      <c r="D955" s="79"/>
     </row>
     <row r="956">
-      <c r="D956" s="72"/>
+      <c r="D956" s="79"/>
     </row>
     <row r="957">
-      <c r="D957" s="72"/>
+      <c r="D957" s="79"/>
     </row>
     <row r="958">
-      <c r="D958" s="72"/>
+      <c r="D958" s="79"/>
     </row>
     <row r="959">
-      <c r="D959" s="72"/>
+      <c r="D959" s="79"/>
     </row>
     <row r="960">
-      <c r="D960" s="72"/>
+      <c r="D960" s="79"/>
     </row>
     <row r="961">
-      <c r="D961" s="72"/>
+      <c r="D961" s="79"/>
     </row>
     <row r="962">
-      <c r="D962" s="72"/>
+      <c r="D962" s="79"/>
     </row>
     <row r="963">
-      <c r="D963" s="72"/>
+      <c r="D963" s="79"/>
     </row>
     <row r="964">
-      <c r="D964" s="72"/>
+      <c r="D964" s="79"/>
     </row>
     <row r="965">
-      <c r="D965" s="72"/>
+      <c r="D965" s="79"/>
     </row>
     <row r="966">
-      <c r="D966" s="72"/>
+      <c r="D966" s="79"/>
     </row>
     <row r="967">
-      <c r="D967" s="72"/>
+      <c r="D967" s="79"/>
     </row>
     <row r="968">
-      <c r="D968" s="72"/>
+      <c r="D968" s="79"/>
     </row>
     <row r="969">
-      <c r="D969" s="72"/>
+      <c r="D969" s="79"/>
     </row>
     <row r="970">
-      <c r="D970" s="72"/>
+      <c r="D970" s="79"/>
     </row>
     <row r="971">
-      <c r="D971" s="72"/>
+      <c r="D971" s="79"/>
     </row>
     <row r="972">
-      <c r="D972" s="72"/>
+      <c r="D972" s="79"/>
     </row>
     <row r="973">
-      <c r="D973" s="72"/>
+      <c r="D973" s="79"/>
     </row>
     <row r="974">
-      <c r="D974" s="72"/>
+      <c r="D974" s="79"/>
     </row>
     <row r="975">
-      <c r="D975" s="72"/>
+      <c r="D975" s="79"/>
     </row>
     <row r="976">
-      <c r="D976" s="72"/>
+      <c r="D976" s="79"/>
     </row>
     <row r="977">
-      <c r="D977" s="72"/>
+      <c r="D977" s="79"/>
     </row>
     <row r="978">
-      <c r="D978" s="72"/>
+      <c r="D978" s="79"/>
     </row>
     <row r="979">
-      <c r="D979" s="72"/>
+      <c r="D979" s="79"/>
     </row>
     <row r="980">
-      <c r="D980" s="72"/>
+      <c r="D980" s="79"/>
     </row>
     <row r="981">
-      <c r="D981" s="72"/>
+      <c r="D981" s="79"/>
     </row>
     <row r="982">
-      <c r="D982" s="72"/>
+      <c r="D982" s="79"/>
     </row>
     <row r="983">
-      <c r="D983" s="72"/>
+      <c r="D983" s="79"/>
     </row>
     <row r="984">
-      <c r="D984" s="72"/>
+      <c r="D984" s="79"/>
     </row>
     <row r="985">
-      <c r="D985" s="72"/>
+      <c r="D985" s="79"/>
     </row>
     <row r="986">
-      <c r="D986" s="72"/>
+      <c r="D986" s="79"/>
     </row>
     <row r="987">
-      <c r="D987" s="72"/>
+      <c r="D987" s="79"/>
     </row>
     <row r="988">
-      <c r="D988" s="72"/>
+      <c r="D988" s="79"/>
     </row>
     <row r="989">
-      <c r="D989" s="72"/>
+      <c r="D989" s="79"/>
     </row>
     <row r="990">
-      <c r="D990" s="72"/>
+      <c r="D990" s="79"/>
     </row>
     <row r="991">
-      <c r="D991" s="72"/>
+      <c r="D991" s="79"/>
     </row>
     <row r="992">
-      <c r="D992" s="72"/>
+      <c r="D992" s="79"/>
     </row>
     <row r="993">
-      <c r="D993" s="72"/>
+      <c r="D993" s="79"/>
     </row>
     <row r="994">
-      <c r="D994" s="72"/>
+      <c r="D994" s="79"/>
     </row>
     <row r="995">
-      <c r="D995" s="72"/>
+      <c r="D995" s="79"/>
     </row>
     <row r="996">
-      <c r="D996" s="72"/>
+      <c r="D996" s="79"/>
     </row>
     <row r="997">
-      <c r="D997" s="72"/>
+      <c r="D997" s="79"/>
     </row>
     <row r="998">
-      <c r="D998" s="72"/>
+      <c r="D998" s="79"/>
     </row>
     <row r="999">
-      <c r="D999" s="72"/>
+      <c r="D999" s="79"/>
     </row>
     <row r="1000">
-      <c r="D1000" s="72"/>
+      <c r="D1000" s="79"/>
     </row>
     <row r="1001">
-      <c r="D1001" s="72"/>
+      <c r="D1001" s="79"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>